<commit_message>
Use search engine local and enhance clean code, + add streaming
</commit_message>
<xml_diff>
--- a/RISTEK.xlsx
+++ b/RISTEK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan\OneDrive\Documents\GitHub\RistekGPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E8BE13-914B-4E33-AE71-7C36D767F341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A55077-309F-4F78-9A3B-B799E28E71EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A966B3A5-28D0-4C85-A779-BF24F350CC49}"/>
   </bookViews>
@@ -42,18 +42,6 @@
     <t>content</t>
   </si>
   <si>
-    <t>How long has RISTEK been operating?</t>
-  </si>
-  <si>
-    <t>What is the primary goal of RISTEK?</t>
-  </si>
-  <si>
-    <t>How does RISTEK contribute to its clients' digital aspirations?</t>
-  </si>
-  <si>
-    <t>Operating for 34 years, RISTEK is an independent organization within the Faculty of Computer Science at Universitas Indonesia. Its mission is to cultivate students’ interest and talent in technology, producing highly skilled individuals in various fields. Serving as the primary hub for students' innovation, RISTEK has developed over 40 products used by tens of thousands annually. The organization has also achieved success in both local and international competitions. Driven by values of excellence, synergy, and equity, RISTEK assists clients in fulfilling their digital aspirations by offering top talents from Universitas Indonesia for their software development needs.</t>
-  </si>
-  <si>
     <t>Our services include:  
 - UI/UX design  
 - Website development  
@@ -71,56 +59,42 @@
 Enjoy personalized service tailored to your needs. We'll collaborate closely with you to ensure the solution we deliver meets your exact specifications.</t>
   </si>
   <si>
-    <t>What are the benefits to collaborate with RISTEK?</t>
-  </si>
-  <si>
-    <t>What are some RISTEK services?</t>
-  </si>
-  <si>
-    <t>What are some RISTEK values?</t>
-  </si>
-  <si>
-    <t>RISTEK Achievements</t>
-  </si>
-  <si>
-    <t>Benefits for RISTEK members</t>
-  </si>
-  <si>
-    <t>Our members benefit from access to the industry's best tools, made possible through collaborations with leading tech partners. These include:
-- Custom Email @ristek.ui.ac.id
-- Zoom Pro Account
-- AWS Credits
-- Google Workspace Account
-- Atlassian PM Tools (Jira, Bitbucket, Confluence)
-- Miro Enterprise Team
-- Notion Education Pro
-- Grammarly Premium
-- Scholarship Plan
-- Sketch Full License
-- Stripe Account
-- DataCamp Learn License</t>
-  </si>
-  <si>
-    <t>What are some RISTEK events?</t>
-  </si>
-  <si>
-    <t>Through our events, we aim to create a lasting impact for participants in their technology exploration journey. Here are some of our recent events:
-- Pekan RISTEK x Google  
-Exclusive Company Visit  
-Participants toured the Google office in Jakarta, with insightful sessions and hands-on implementation of Google Cloud Platform by industry professionals.
-- RISTEK x Ziliun Classss  
-UI/UX and Career Workshop  
-Workipedia Class: Spill the Tech, a collaboration program between Ziliun and Telkomsel, introduced the tech industry to university students through RISTEK with Online Career Talk and Mini Workshops.
-- RISTEK x tiket.com  
-Exclusive Company Visit  
-The RISTEK team visited the headquarters of Indonesia's OTA giant, tiket.com, for an exclusive networking session and office tour.
-- RISTEK Sisters in Tech  
-A pioneering women-only tech mentorship program open for female Indonesian citizens ages 17-25, offering mentorship in Product Management, UI/UX Design, Software Engineering, and Data Analytics.
-- Pekan RISTEK  
-An annual event showcasing RISTEK to Fasilkom UI students through open classes and competitions hosted by Special Interest Groups, including Data Science, Project Management, Digital Product Design, and Web Development.</t>
-  </si>
-  <si>
-    <t>RISTEK projects</t>
+    <t>How long has RISTEK Fasilkom UI been operating?</t>
+  </si>
+  <si>
+    <t>Operating for 34 years, RISTEK Fasilkom UI is an independent organization within the Faculty of Computer Science at Universitas Indonesia. Its mission is to cultivate students’ interest and talent in technology, producing highly skilled individuals in various fields. Serving as the primary hub for students' innovation, RISTEK Fasilkom UI has developed over 40 products used by tens of thousands annually. The organization has also achieved success in both local and international competitions. Driven by values of excellence, synergy, and equity, RISTEK Fasilkom UI assists clients in fulfilling their digital aspirations by offering top talents from Universitas Indonesia for their software development needs.</t>
+  </si>
+  <si>
+    <t>What is the primary goal of RISTEK Fasilkom UI?</t>
+  </si>
+  <si>
+    <t>How does RISTEK Fasilkom UI contribute to its clients' digital aspirations?</t>
+  </si>
+  <si>
+    <t>What is RISTEK Fasilkom UI</t>
+  </si>
+  <si>
+    <t>What are the benefits to collaborate with RISTEK Fasilkom UI?</t>
+  </si>
+  <si>
+    <t>Why Collaborate with RISTEK Fasilkom UI?</t>
+  </si>
+  <si>
+    <t>What are some RISTEK Fasilkom UI services?</t>
+  </si>
+  <si>
+    <t>What are some RISTEK Fasilkom UI values?</t>
+  </si>
+  <si>
+    <t>We strive for excellence
+- By creating an ambition-fueled environment, we encourage every member to continually improve and achieve their best individually, thus contributing to the acceleration of RISTEK Fasilkom UI’s growth collectively.
+We build strong synergies
+- Purposeful partnerships with external entities and effective collaboration across internal teams act as catalysts for us to achieve our mission.
+We aim to achieve equity
+- Along with the purpose to provide equal opportunities &amp; resources to each member, we are committed to support them to grow to their maximum potential.</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI Achievements</t>
   </si>
   <si>
     <t>Overall achievements:
@@ -133,22 +107,22 @@
 Here are some specific achievements that validate our prowess in the field of technology:
 **Competitions:**
 - Over the years, our members have conquered numerous IT competitions nationwide, bringing pride to our organization.
-**People Operations Ristek:**
+**People Operations RISTEK Fasilkom UI:**
 - Successfully resolved conflicts between members.
 - Managed to run the entire division program.
 - Achieved a member satisfaction rate of 4.4/5.0.
-**Product Office Ristek:**
+**Product Office RISTEK Fasilkom UI:**
 - Revamped Susun Jadwal.
 **Project Management:**
 - Successfully managed 20+ projects in the past year.
 - Generated Rp200million+ of project value.
-**Web Development Ristek:**
+**Web Development RISTEK Fasilkom UI:**
 - Revamped Susun Jadwal.
 - Launched PMB 2022.
-- Launched RISTEK 2022.
-**Mobile &amp; Web Development &amp; Product Office Ristek:**
+- Launched RISTEK Fasilkom UI 2022.
+**Mobile &amp; Web Development &amp; Product Office RISTEK Fasilkom UI:**
 - Launched Ulas Kelas.
-**Mobile Development Ristek:**
+**Mobile Development RISTEK Fasilkom UI:**
 - Reached over 100M+ project value from multiple top companies.
 **Achievements in Competitions:**
 - 2nd place in UX Design Competition (Gemastik XV).
@@ -166,42 +140,98 @@
 - 5th place in Technicality (Gemastik XIV).
 - Semifinalist in Green Gamejam (Green Gamejam, 2022).
 **Other Achievements:**
-- Established the first women-only tech mentorship program, RISTEK Sisters in Tech (SisTech), with 1,350+ applicants.
+- Established the first women-only tech mentorship program, RISTEK Fasilkom UI Sisters in Tech (SisTech), with 1,350+ applicants.
 - Secured a partnership deal with Datacamp.
 - Arranged company visits to Tiket.com and Google.
 - Gained over 2500+ followers on Instagram.
-- Successfully managed 5 Ristek’s Social Media.
+- Successfully managed 5 RISTEK Fasilkom UI’s Social Media.
 - Achieved a 93% satisfaction rate in copywriting and design.</t>
   </si>
   <si>
-    <t>RISTEK contact</t>
+    <t>Benefits for RISTEK Fasilkom UI members</t>
+  </si>
+  <si>
+    <t>Our members benefit from access to the industry's best tools, made possible through collaborations with leading tech partners. These include:
+- Custom Email @RISTEK Fasilkom UI.ui.ac.id
+- Zoom Pro Account
+- AWS Credits
+- Google Workspace Account
+- Atlassian PM Tools (Jira, Bitbucket, Confluence)
+- Miro Enterprise Team
+- Notion Education Pro
+- Grammarly Premium
+- Scholarship Plan
+- Sketch Full License
+- Stripe Account
+- DataCamp Learn License</t>
+  </si>
+  <si>
+    <t>What are some RISTEK Fasilkom UI events?</t>
+  </si>
+  <si>
+    <t>Through our events, we aim to create a lasting impact for participants in their technology exploration journey. Here are some of our recent events:
+- Pekan RISTEK Fasilkom UI x Google  
+Exclusive Company Visit  
+Participants toured the Google office in Jakarta, with insightful sessions and hands-on implementation of Google Cloud Platform by industry professionals.
+- RISTEK Fasilkom UI x Ziliun Classss  
+UI/UX and Career Workshop  
+Workipedia Class: Spill the Tech, a collaboration program between Ziliun and Telkomsel, introduced the tech industry to university students through RISTEK Fasilkom UI with Online Career Talk and Mini Workshops.
+- RISTEK Fasilkom UI x tiket.com  
+Exclusive Company Visit  
+The RISTEK Fasilkom UI team visited the headquarters of Indonesia's OTA giant, tiket.com, for an exclusive networking session and office tour.
+- RISTEK Fasilkom UI Sisters in Tech  
+A pioneering women-only tech mentorship program open for female Indonesian citizens ages 17-25, offering mentorship in Product Management, UI/UX Design, Software Engineering, and Data Analytics.
+- Pekan RISTEK Fasilkom UI  
+An annual event showcasing RISTEK Fasilkom UI to Fasilkom UI students through open classes and competitions hosted by Special Interest Groups, including Data Science, Project Management, Digital Product Design, and Web Development.</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI link</t>
+  </si>
+  <si>
+    <t>Here's a showcase of our past projects and capabilities:
+Past Projects:
+- UlasKelas: A mobile application designed to assist students in learning about available courses.
+https://github.com/RISTEK Fasilkom UIoss/ulaskelas-frontend
+https://play.google.com/store/apps/details?id=com.RISTEK Fasilkom UI.ulaskelas&amp;hl=en
+- SusunJadwal: The #1 app for helping University of Indonesia students plan courses and share schedules, with over 200k annual users.
+https://github.com/RISTEK Fasilkom UIoss/susunjadwal-frontend
+http://susunjadwal.cs.ui.ac.id/
+- RISTEK Fasilkom UI.LINK: An easy-to-use, customizable URL shortener, offering quick and free service without requiring registration.
+https://github.com/RISTEK Fasilkom UIoss/RISTEK Fasilkom UI-link
+https://RISTEK Fasilkom UI.link/</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI susun jadwal</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI Ulas Kelas</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI products</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI projects</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI contact</t>
   </si>
   <si>
     <t>Location:
 Universitas Indonesia, Depok
-About RISTEK:
-RISTEK is a student-founded non-profit organization from Universitas Indonesia's Faculty of Computer Science, supported by a United States of America 501(c)(3) non-profit.
+About RISTEK Fasilkom UI:
+RISTEK Fasilkom UI is a student-founded non-profit organization from Universitas Indonesia's Faculty of Computer Science, supported by a United States of America 501(c)(3) non-profit.
 Contact:
-Email: team@ristek.cs.ui.ac.id
+Email: team@RISTEK Fasilkom UI.cs.ui.ac.id
 Official Learning Partner:
 Gojek, GoTo Learning Partner
 Accelerated by:
 Hack+</t>
   </si>
   <si>
-    <t>Why Collaborate with RISTEK?</t>
-  </si>
-  <si>
-    <t>RISTEK Ulas Kelas</t>
-  </si>
-  <si>
-    <t>RISTEK link</t>
-  </si>
-  <si>
-    <t>RISTEK susun jadwal</t>
-  </si>
-  <si>
-    <t>RISTEK location</t>
+    <t>RISTEK Fasilkom UI location</t>
+  </si>
+  <si>
+    <t>What are RISTEK Fasilkom UI divisions?</t>
   </si>
   <si>
     <t>Our members are a part of diverse divisions that work together as one.
@@ -219,7 +249,7 @@
 Explore your interest and capabilities in developing your game with Game Development. You will have the chance to improve your skills in developing games by using popular game engines. By learning the aspects of game design, the basics of coding patterns, and implementing state machines in game development, you will be able to work as a team in developing games by joining Game Development.
 People Operations
 About Us
-People Operations is the baseline of all RISTEK’s divisions.People Operations aims to encourage and cultivate every member of RISTEK. People Operations will make sure that every member gains every value RISTEK has to offer. Together with your division, you’ll create an impactful team that will give you not only soft skill benefits but also a hands-on learning experience.
+People Operations is the baseline of all RISTEK Fasilkom UI’s divisions.People Operations aims to encourage and cultivate every member of RISTEK Fasilkom UI. People Operations will make sure that every member gains every value RISTEK Fasilkom UI has to offer. Together with your division, you’ll create an impactful team that will give you not only soft skill benefits but also a hands-on learning experience.
 Mobile Development
 About Us
 Learn about the development of mobile applications from zero with Mobile Development. This year we will focus on Flutter and Kotlin - new mobile application frameworks recommended by Google. You will start from the basics: Dart and Kotlin programming language, a paradigm in mobile development, and get used to the best practices of mobile development. Eventually, you will be able to develop fully functional and refreshing mobile applications by joining Mobile Development.
@@ -228,49 +258,19 @@
 Learn about cybersecurity happening in the real world with Network Security and Operating System. You will start from the essentials: cybersecurity, operating system, and networking, then escalate it to some advanced trick on bypassing a firewall. Be prepared to dig deeper to cyber's iceberg and realize that no system is safe.
 Project Management
 About Us
-Project Management is where RISTEK’s internal and external projects are managed. In Project Management, you will learn how to be a professional project manager equipped with soft and technical skills. Project Management focused on handling each project with shared responsibilities on implementing the project life cycle. Here you will take part as a project manager of a team consisting of brilliant individuals to ensure the project has a set direction of a successful outcome.
+Project Management is where RISTEK Fasilkom UI’s internal and external projects are managed. In Project Management, you will learn how to be a professional project manager equipped with soft and technical skills. Project Management focused on handling each project with shared responsibilities on implementing the project life cycle. Here you will take part as a project manager of a team consisting of brilliant individuals to ensure the project has a set direction of a successful outcome.
 Strategic Partnerships
 About Us
-Strategic Partnerships is responsible for building and maintaining relationships with companies, organizations, and other entities that can provide mutually-beneficial opportunities for RISTEK and its members through meaningful collaboration and initiatives.
+Strategic Partnerships is responsible for building and maintaining relationships with companies, organizations, and other entities that can provide mutually-beneficial opportunities for RISTEK Fasilkom UI and its members through meaningful collaboration and initiatives.
 Web Development
 About Us
 Get valuable and career-kickstarting web development knowledge with Web Development. You will learn the best practices of web development skills and have the opportunity to build up your portfolio. Through internal classes, you will learn about the best practices of web development skills such as analytical skills software engineering implementation, various technology stacks that suits right now industry and many more! You will be provided with mentors that also conducts routine 1 on 1 session to help track your web development skill progress and also opportunity to work on real projects!
 Marketing and Communications
 About Us
-Marketing &amp; Communications focuses on promoting RISTEK as an organization by developing and executing marketing strategies to communicate RISTEK’s values and increase brand awareness.
+Marketing &amp; Communications focuses on promoting RISTEK Fasilkom UI as an organization by developing and executing marketing strategies to communicate RISTEK Fasilkom UI’s values and increase brand awareness.
 Product Operations
 About Us
 Product Operations (referred to as Product Ops) is a part of the Product Office team. As a member of Product Ops, you will be a part of an independent team directly under the Executive Director of Product.</t>
-  </si>
-  <si>
-    <t>What are RISTEK divisions?</t>
-  </si>
-  <si>
-    <t>We strive for excellence
-- By creating an ambition-fueled environment, we encourage every member to continually improve and achieve their best individually, thus contributing to the acceleration of RISTEK’s growth collectively.
-We build strong synergies
-- Purposeful partnerships with external entities and effective collaboration across internal teams act as catalysts for us to achieve our mission.
-We aim to achieve equity
-- Along with the purpose to provide equal opportunities &amp; resources to each member, we are committed to support them to grow to their maximum potential.</t>
-  </si>
-  <si>
-    <t>Here's a showcase of our past projects and capabilities:
-Past Projects:
-- UlasKelas: A mobile application designed to assist students in learning about available courses.
-https://github.com/ristekoss/ulaskelas-frontend
-https://play.google.com/store/apps/details?id=com.ristek.ulaskelas&amp;hl=en
-- SusunJadwal: The #1 app for helping University of Indonesia students plan courses and share schedules, with over 200k annual users.
-https://github.com/ristekoss/susunjadwal-frontend
-http://susunjadwal.cs.ui.ac.id/
-- RISTEK.LINK: An easy-to-use, customizable URL shortener, offering quick and free service without requiring registration.
-https://github.com/ristekoss/ristek-link
-https://ristek.link/</t>
-  </si>
-  <si>
-    <t>What is RISTEK</t>
-  </si>
-  <si>
-    <t>RISTEK products</t>
   </si>
 </sst>
 </file>
@@ -311,7 +311,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,7 +631,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -648,7 +650,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -656,7 +658,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -664,7 +666,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -672,130 +674,130 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add alternative mistral llm and fix minor and add data
</commit_message>
<xml_diff>
--- a/RISTEK.xlsx
+++ b/RISTEK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan\OneDrive\Documents\GitHub\RistekGPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A55077-309F-4F78-9A3B-B799E28E71EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97CE318-EF46-4F65-B9C7-585969A4BEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A966B3A5-28D0-4C85-A779-BF24F350CC49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>title</t>
   </si>
@@ -65,25 +65,10 @@
     <t>Operating for 34 years, RISTEK Fasilkom UI is an independent organization within the Faculty of Computer Science at Universitas Indonesia. Its mission is to cultivate students’ interest and talent in technology, producing highly skilled individuals in various fields. Serving as the primary hub for students' innovation, RISTEK Fasilkom UI has developed over 40 products used by tens of thousands annually. The organization has also achieved success in both local and international competitions. Driven by values of excellence, synergy, and equity, RISTEK Fasilkom UI assists clients in fulfilling their digital aspirations by offering top talents from Universitas Indonesia for their software development needs.</t>
   </si>
   <si>
-    <t>What is the primary goal of RISTEK Fasilkom UI?</t>
-  </si>
-  <si>
     <t>How does RISTEK Fasilkom UI contribute to its clients' digital aspirations?</t>
   </si>
   <si>
     <t>What is RISTEK Fasilkom UI</t>
-  </si>
-  <si>
-    <t>What are the benefits to collaborate with RISTEK Fasilkom UI?</t>
-  </si>
-  <si>
-    <t>Why Collaborate with RISTEK Fasilkom UI?</t>
-  </si>
-  <si>
-    <t>What are some RISTEK Fasilkom UI services?</t>
-  </si>
-  <si>
-    <t>What are some RISTEK Fasilkom UI values?</t>
   </si>
   <si>
     <t>We strive for excellence
@@ -95,6 +80,113 @@
   </si>
   <si>
     <t>RISTEK Fasilkom UI Achievements</t>
+  </si>
+  <si>
+    <t>Benefits for RISTEK Fasilkom UI members</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI susun jadwal</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI Ulas Kelas</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI products</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI projects</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI contact</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI location</t>
+  </si>
+  <si>
+    <t>Our members are a part of diverse divisions that work together as one.
+Executive Fellows
+About Us
+Executive Fellows function as our leadership board in setting the firm’s directions, policies, and strategic goals. It includes the managing directors and directors of product, administrations, and finance.
+Data Science
+About Us
+Data Science will give you exposure to what data scientists do daily, such as data wrangling, manipulation, modeling, to produce meaningful insights for strategic decision making. This year, Data Science will focus more on the practical side of data science, easily applicable in a wide range of data science-related tasks. We believe that taking part in this highly-achieving community will allow you to grow and maximize your potential in the field of data. If you are interested in analyzing data, programming, statistics, and working with actual data, Data Science is for you!
+Digital Product Design
+About Us
+Digital Product Design is the right place for you for those who are passionate about designing a product. In designing those products, you will learn how to use the UI/UX principles correctly and research the user problems directly. This year, Digital Product Design aims to collaborate with Web Development to produce digital products with interactive and attractive designs and a good user experience. Here, you have the chance to build your design portfolio that will be useful for your future product design career.
+Game Development
+About Us
+Explore your interest and capabilities in developing your game with Game Development. You will have the chance to improve your skills in developing games by using popular game engines. By learning the aspects of game design, the basics of coding patterns, and implementing state machines in game development, you will be able to work as a team in developing games by joining Game Development.
+People Operations
+About Us
+People Operations is the baseline of all RISTEK Fasilkom UI’s divisions.People Operations aims to encourage and cultivate every member of RISTEK Fasilkom UI. People Operations will make sure that every member gains every value RISTEK Fasilkom UI has to offer. Together with your division, you’ll create an impactful team that will give you not only soft skill benefits but also a hands-on learning experience.
+Mobile Development
+About Us
+Learn about the development of mobile applications from zero with Mobile Development. This year we will focus on Flutter and Kotlin - new mobile application frameworks recommended by Google. You will start from the basics: Dart and Kotlin programming language, a paradigm in mobile development, and get used to the best practices of mobile development. Eventually, you will be able to develop fully functional and refreshing mobile applications by joining Mobile Development.
+Network, Security, OS
+About Us
+Learn about cybersecurity happening in the real world with Network Security and Operating System. You will start from the essentials: cybersecurity, operating system, and networking, then escalate it to some advanced trick on bypassing a firewall. Be prepared to dig deeper to cyber's iceberg and realize that no system is safe.
+Project Management
+About Us
+Project Management is where RISTEK Fasilkom UI’s internal and external projects are managed. In Project Management, you will learn how to be a professional project manager equipped with soft and technical skills. Project Management focused on handling each project with shared responsibilities on implementing the project life cycle. Here you will take part as a project manager of a team consisting of brilliant individuals to ensure the project has a set direction of a successful outcome.
+Strategic Partnerships
+About Us
+Strategic Partnerships is responsible for building and maintaining relationships with companies, organizations, and other entities that can provide mutually-beneficial opportunities for RISTEK Fasilkom UI and its members through meaningful collaboration and initiatives.
+Web Development
+About Us
+Get valuable and career-kickstarting web development knowledge with Web Development. You will learn the best practices of web development skills and have the opportunity to build up your portfolio. Through internal classes, you will learn about the best practices of web development skills such as analytical skills software engineering implementation, various technology stacks that suits right now industry and many more! You will be provided with mentors that also conducts routine 1 on 1 session to help track your web development skill progress and also opportunity to work on real projects!
+Marketing and Communications
+About Us
+Marketing &amp; Communications focuses on promoting RISTEK Fasilkom UI as an organization by developing and executing marketing strategies to communicate RISTEK Fasilkom UI’s values and increase brand awareness.
+Product Operations
+About Us
+Product Operations (referred to as Product Ops) is a part of the Product Office team. As a member of Product Ops, you will be a part of an independent team directly under the Executive Director of Product.</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI ristek.link</t>
+  </si>
+  <si>
+    <t>Here's a showcase of our past projects and capabilities:
+Past Projects:
+- UlasKelas: A mobile application designed to assist students in learning about available courses.
+https://github.com/ristekoss/ulaskelas-frontend
+https://play.google.com/store/apps/details?id=com.ristek.ulaskelas&amp;hl=en
+- SusunJadwal: The #1 app for helping University of Indonesia students plan courses and share schedules, with over 200k annual users.
+https://github.com/ristekoss/susunjadwal-frontend
+http://susunjadwal.cs.ui.ac.id/
+- RISTEK.LINK: An easy-to-use, customizable URL shortener, offering quick and free service without requiring registration.
+https://github.com/ristekoss/ristek-link
+https://ristek.link/</t>
+  </si>
+  <si>
+    <t>Through our events, we aim to create a lasting impact for participants in their technology exploration journey. Here are some of our recent events:
+- Pekan RISTEK x Google  
+Exclusive Company Visit  
+Participants toured the Google office in Jakarta, with insightful sessions and hands-on implementation of Google Cloud Platform by industry professionals.
+- RISTEK Fasilkom UI x Ziliun Classss  
+UI/UX and Career Workshop  
+Workipedia Class: Spill the Tech, a collaboration program between Ziliun and Telkomsel, introduced the tech industry to university students through RISTEK Fasilkom UI with Online Career Talk and Mini Workshops.
+- RISTEK Fasilkom UI x tiket.com  
+Exclusive Company Visit  
+The RISTEK Fasilkom UI team visited the headquarters of Indonesia's OTA giant, tiket.com, for an exclusive networking session and office tour.
+- RISTEK Fasilkom UI Sisters in Tech  
+A pioneering women-only tech mentorship program open for female Indonesian citizens ages 17-25, offering mentorship in Product Management, UI/UX Design, Software Engineering, and Data Analytics.
+- Pekan RISTEK
+An annual event showcasing RISTEK Fasilkom UI to Fasilkom UI students through open classes and competitions hosted by Special Interest Groups, including Data Science, Project Management, Digital Product Design, and Web Development.</t>
+  </si>
+  <si>
+    <t>Our members benefit from access to the industry's best tools, made possible through collaborations with leading tech partners. These include:
+- Custom Email @ristek.ui.ac.id
+- Zoom Pro Account
+- AWS Credits
+- Google Workspace Account
+- Atlassian PM Tools (Jira, Bitbucket, Confluence)
+- Miro Enterprise Team
+- Notion Education Pro
+- Grammarly Premium
+- Scholarship Plan
+- Sketch Full License
+- Stripe Account
+- DataCamp Learn License</t>
   </si>
   <si>
     <t>Overall achievements:
@@ -140,7 +232,7 @@
 - 5th place in Technicality (Gemastik XIV).
 - Semifinalist in Green Gamejam (Green Gamejam, 2022).
 **Other Achievements:**
-- Established the first women-only tech mentorship program, RISTEK Fasilkom UI Sisters in Tech (SisTech), with 1,350+ applicants.
+- Established the first women-only tech mentorship program, RISTEK Sisters in Tech (SisTech), with 1,350+ applicants.
 - Secured a partnership deal with Datacamp.
 - Arranged company visits to Tiket.com and Google.
 - Gained over 2500+ followers on Instagram.
@@ -148,129 +240,540 @@
 - Achieved a 93% satisfaction rate in copywriting and design.</t>
   </si>
   <si>
-    <t>Benefits for RISTEK Fasilkom UI members</t>
-  </si>
-  <si>
-    <t>Our members benefit from access to the industry's best tools, made possible through collaborations with leading tech partners. These include:
-- Custom Email @RISTEK Fasilkom UI.ui.ac.id
-- Zoom Pro Account
-- AWS Credits
-- Google Workspace Account
-- Atlassian PM Tools (Jira, Bitbucket, Confluence)
-- Miro Enterprise Team
-- Notion Education Pro
-- Grammarly Premium
-- Scholarship Plan
-- Sketch Full License
-- Stripe Account
-- DataCamp Learn License</t>
-  </si>
-  <si>
-    <t>What are some RISTEK Fasilkom UI events?</t>
-  </si>
-  <si>
-    <t>Through our events, we aim to create a lasting impact for participants in their technology exploration journey. Here are some of our recent events:
-- Pekan RISTEK Fasilkom UI x Google  
-Exclusive Company Visit  
-Participants toured the Google office in Jakarta, with insightful sessions and hands-on implementation of Google Cloud Platform by industry professionals.
-- RISTEK Fasilkom UI x Ziliun Classss  
-UI/UX and Career Workshop  
-Workipedia Class: Spill the Tech, a collaboration program between Ziliun and Telkomsel, introduced the tech industry to university students through RISTEK Fasilkom UI with Online Career Talk and Mini Workshops.
-- RISTEK Fasilkom UI x tiket.com  
-Exclusive Company Visit  
-The RISTEK Fasilkom UI team visited the headquarters of Indonesia's OTA giant, tiket.com, for an exclusive networking session and office tour.
-- RISTEK Fasilkom UI Sisters in Tech  
-A pioneering women-only tech mentorship program open for female Indonesian citizens ages 17-25, offering mentorship in Product Management, UI/UX Design, Software Engineering, and Data Analytics.
-- Pekan RISTEK Fasilkom UI  
-An annual event showcasing RISTEK Fasilkom UI to Fasilkom UI students through open classes and competitions hosted by Special Interest Groups, including Data Science, Project Management, Digital Product Design, and Web Development.</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI link</t>
-  </si>
-  <si>
-    <t>Here's a showcase of our past projects and capabilities:
-Past Projects:
-- UlasKelas: A mobile application designed to assist students in learning about available courses.
-https://github.com/RISTEK Fasilkom UIoss/ulaskelas-frontend
-https://play.google.com/store/apps/details?id=com.RISTEK Fasilkom UI.ulaskelas&amp;hl=en
-- SusunJadwal: The #1 app for helping University of Indonesia students plan courses and share schedules, with over 200k annual users.
-https://github.com/RISTEK Fasilkom UIoss/susunjadwal-frontend
-http://susunjadwal.cs.ui.ac.id/
-- RISTEK Fasilkom UI.LINK: An easy-to-use, customizable URL shortener, offering quick and free service without requiring registration.
-https://github.com/RISTEK Fasilkom UIoss/RISTEK Fasilkom UI-link
-https://RISTEK Fasilkom UI.link/</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI susun jadwal</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI Ulas Kelas</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI products</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI projects</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI contact</t>
-  </si>
-  <si>
     <t>Location:
 Universitas Indonesia, Depok
 About RISTEK Fasilkom UI:
 RISTEK Fasilkom UI is a student-founded non-profit organization from Universitas Indonesia's Faculty of Computer Science, supported by a United States of America 501(c)(3) non-profit.
 Contact:
-Email: team@RISTEK Fasilkom UI.cs.ui.ac.id
+Email: team@ristek.cs.ui.ac.id
 Official Learning Partner:
 Gojek, GoTo Learning Partner
 Accelerated by:
 Hack+</t>
   </si>
   <si>
-    <t>RISTEK Fasilkom UI location</t>
-  </si>
-  <si>
-    <t>What are RISTEK Fasilkom UI divisions?</t>
-  </si>
-  <si>
-    <t>Our members are a part of diverse divisions that work together as one.
-Executive Fellows
-About Us
-Executive Fellows function as our leadership board in setting the firm’s directions, policies, and strategic goals. It includes the managing directors and directors of product, administrations, and finance.
-Data Science
-About Us
-Data Science will give you exposure to what data scientists do daily, such as data wrangling, manipulation, modeling, to produce meaningful insights for strategic decision making. This year, Data Science will focus more on the practical side of data science, easily applicable in a wide range of data science-related tasks. We believe that taking part in this highly-achieving community will allow you to grow and maximize your potential in the field of data. If you are interested in analyzing data, programming, statistics, and working with actual data, Data Science is for you!
-Digital Product Design
-About Us
-Digital Product Design is the right place for you for those who are passionate about designing a product. In designing those products, you will learn how to use the UI/UX principles correctly and research the user problems directly. This year, Digital Product Design aims to collaborate with Web Development to produce digital products with interactive and attractive designs and a good user experience. Here, you have the chance to build your design portfolio that will be useful for your future product design career.
-Game Development
-About Us
-Explore your interest and capabilities in developing your game with Game Development. You will have the chance to improve your skills in developing games by using popular game engines. By learning the aspects of game design, the basics of coding patterns, and implementing state machines in game development, you will be able to work as a team in developing games by joining Game Development.
-People Operations
-About Us
-People Operations is the baseline of all RISTEK Fasilkom UI’s divisions.People Operations aims to encourage and cultivate every member of RISTEK Fasilkom UI. People Operations will make sure that every member gains every value RISTEK Fasilkom UI has to offer. Together with your division, you’ll create an impactful team that will give you not only soft skill benefits but also a hands-on learning experience.
-Mobile Development
-About Us
-Learn about the development of mobile applications from zero with Mobile Development. This year we will focus on Flutter and Kotlin - new mobile application frameworks recommended by Google. You will start from the basics: Dart and Kotlin programming language, a paradigm in mobile development, and get used to the best practices of mobile development. Eventually, you will be able to develop fully functional and refreshing mobile applications by joining Mobile Development.
-Network, Security, OS
-About Us
-Learn about cybersecurity happening in the real world with Network Security and Operating System. You will start from the essentials: cybersecurity, operating system, and networking, then escalate it to some advanced trick on bypassing a firewall. Be prepared to dig deeper to cyber's iceberg and realize that no system is safe.
-Project Management
-About Us
-Project Management is where RISTEK Fasilkom UI’s internal and external projects are managed. In Project Management, you will learn how to be a professional project manager equipped with soft and technical skills. Project Management focused on handling each project with shared responsibilities on implementing the project life cycle. Here you will take part as a project manager of a team consisting of brilliant individuals to ensure the project has a set direction of a successful outcome.
-Strategic Partnerships
-About Us
-Strategic Partnerships is responsible for building and maintaining relationships with companies, organizations, and other entities that can provide mutually-beneficial opportunities for RISTEK Fasilkom UI and its members through meaningful collaboration and initiatives.
-Web Development
-About Us
-Get valuable and career-kickstarting web development knowledge with Web Development. You will learn the best practices of web development skills and have the opportunity to build up your portfolio. Through internal classes, you will learn about the best practices of web development skills such as analytical skills software engineering implementation, various technology stacks that suits right now industry and many more! You will be provided with mentors that also conducts routine 1 on 1 session to help track your web development skill progress and also opportunity to work on real projects!
-Marketing and Communications
-About Us
-Marketing &amp; Communications focuses on promoting RISTEK Fasilkom UI as an organization by developing and executing marketing strategies to communicate RISTEK Fasilkom UI’s values and increase brand awareness.
-Product Operations
-About Us
-Product Operations (referred to as Product Ops) is a part of the Product Office team. As a member of Product Ops, you will be a part of an independent team directly under the Executive Director of Product.</t>
+    <t>#201-250 in Computer Science &amp; Information Systems in the world (QS WUR 2022)
+#21 in Competitive Programming in the world (ICPC 2019 World Finals)
+#1 Best University in Indonesia (THE WUR 2022)
+#1 Juara Umum GEMASTIK (GEMASTIK 2016-2020)</t>
+  </si>
+  <si>
+    <t>Fasilkom UI overall achievements</t>
+  </si>
+  <si>
+    <t>Sejarah Fakultas Ilmu Komputer Universitas Indonesia (Fasilkom UI) adalah tempat yang menantang orang-orang dengan rasa ingin tahu yang tinggi dan bersemangat untuk berimajinasi dan berkarya di bidang ilmu komputer dan sistem informasi. Fasilkom UI merupakan salah satu institusi pendidikan tinggi terbaik di dunia dalam bidang ilmu komputer dan sistem informasi. Dengan riset yang mutakhir, start-up inovatif, ambisi yang besar, pembelajaran yang hands-on, dan robot-robot pintar, Fasilkom UI tidak hanya membayangkan masa depan, tapi juga turut membuatnya.
+1972 - Sejarah Fakultas Ilmu Komputer Universitas Indonesia tidak dapat dipisahkan dari pendirian Pusat Ilmu Komputer Universitas Indonesia (Pusilkom UI) pada tahun 1972.
+1986 - Berangkat dari desakan dari berbagai pihak kepada UI untuk menyelenggarakan program pendidikan ilmu komputer, maka pada tahun 1986 Pusilkom UI mulai menyelenggarakan program studi ilmu komputer untuk jenjang sarjana.
+1988 - Mengikuti perkembangan dan permintaan akan program studi yang mendalami ilmu komputer pada level yang lebih tinggi, Pusilkom UI resmi membuka program studi Magister Ilmu Komputer pada tahun 1988.
+1993 - Semua program studi yang sudah ada kemudian bernaung di bawah Fakultas Ilmu Komputer UI (Fasilkom UI) yang secara resmi terbentuk pada tahun 1993.
+1996 - Program studi Magister Teknologi Informasi (MTI) resmi dibuka. Perkuliahan MTI di kampus UI Salemba.
+1998 - Menjelang akhir milenium, Fasilkom UI memulai program doktor ilmu komputer pertama di Indonesia pada tahun 1998.
+2002 - Menanggapi permintaan akan talenta ilmu komputer dengan wawasan global, Fasilkom UI membuka program studi ilmu komputer kelas internasional.
+2007 - Seiring dengan meningkatnya peran ilmu komputer dalam konteks organisasi, Fasilkom UI membuka program studi Sistem Informasi dan Program Parelel Lanjutan D3 (Ekstensi) Sistem Informasi.</t>
+  </si>
+  <si>
+    <t>Sejarah Fasilkom UI</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI divisions</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI events</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI values</t>
+  </si>
+  <si>
+    <t>RISTEK Fasilkom UI services</t>
+  </si>
+  <si>
+    <t>Benefits to collaborate with RISTEK Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Reason to Collaborate with RISTEK Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Primary goal of RISTEK Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Visi
+Fakultas Ilmu Komputer UI sebagai pusat unggulan di bidang Ilmu Komputer dan Teknologi Informasi di Indonesia yang diakui oleh masyarakat ilmiah internasional, sehat secara organisasi dan berkontribusi secara nyata pada peningkatan daya saing bangsa Indonesia.
+Visi ini mengandung makna bahwa Fasilkom UI bertekad menjadi "top referral" bagi perkembangan ilmu komputer dan teknologi informasi di Indonesia. Artinya, Fasilkom UI harus menjadi institusi terdepan dalam mengembangkan ilmu komputer dan teknologi informasi di Indonesia.
+Visi ini dipilih karena secara historis, Fasilkom yang lahir dari Pusilkom merupakan institusi pertama di Indonesia yang berkecimpung dalam bidang ilmu komputer. Disamping itu, sumber daya yang dimiliki sangat memadai untuk menjadi institusi yang mampu bersaing di tingkat internasional.
+Misi
+Pendidikan
+Menghasilkan lulusan yang mampu bersaing dengan kompetitif, tidak hanya dalam pasar lokal, namun juga global.
+Penelitian &amp; Pelayanan
+Menciptakan, mengembangkan dan menerapkan ilmu pengetahuan dan teknologi untuk peningkatan daya saing bangsa.
+Program Penjangkauan
+Bertanggung jawab secara moral dan sosial pada pengembangan kecerdasan dan martabat bangsa.
+Budaya Organisasi
+Bersama membangun layanan prima, cerdas dan berkualitas dengan motto "Excellence in Teamwork". Fasilkom UI merancang kegiatan akademik yang terpadu antara Pendidikan, Penelitian &amp; Pelayanan, dan Program Penjangkauan. Segenap sumber daya dikerahkan untuk menunjang tiga aspek kegiatan akademik tersebut.</t>
+  </si>
+  <si>
+    <t>Visi dan Misi Fasilkom UI</t>
+  </si>
+  <si>
+    <t>PROGRAM SARJANA
+Program Studi Ilmu Komputer
+GELAR
+Sarjana Ilmu Komputer (S. Kom)
+LOKASI KAMPUS
+Kampus UI Depok
+JADWAL PERKULIAHAN
+Pagi/Hari Kerja
+LAMA STUDI
+8 Semester (144 SKS)
+BAHASA
+Indonesia
+AKREDITASI
+UNGGUL oleh lembaga akreditasi Indonesian Accreditation Board for Engineering Education (IABEE)
+cs.ui.ac.id/sik
+Program Studi Sarjana Ilmu Komputer di bawah naungan Fakultas Ilmu Komputer Universitas Indonesia (Fasilkom UI) terdiri dari program reguler dan program non reguler. Program ini memberikan kesempatan kepada para lulusan SMA/sederajat yang terbaik untuk mendapatkan pendidikan dan keahlian di bidang Ilmu Komputer pada tingkat sarjana. Program ini dirancang untuk memenuhi kebutuhan tenaga-tenaga yang terampil dan profesional di bidang Ilmu Komputer khususnya. Dengan pengalamannya selama lebih dari 30 tahun, Program Studi Sarjana Ilmu Komputer telah diakui kemampuan dan kualitasnya dalam memberikan pendidikan pada jenjang sarjana di bidang Ilmu Komputer.
+Program Studi Sarjana Ilmu Komputer menawarkan keseimbangan antara fondasi keilmuan yang kokoh di bidang Ilmu Komputer dan keterampilan profesional dalam bidang Ilmu Komputer di antaranya matematika diskret, pemrograman, struktur data &amp; algoritma, arsitektur komputer, basis data, sistem operasi, jaringan komputer, teori komputasi, rekayasa perangkat lunak, serta sistem cerdas. Untuk pengembangan keterampilan profesional, Program Studi Sarjana Ilmu Komputer menawarkan berbagai mata kuliah terapan yang dapat digolongkan ke dalam beberapa peminatan:
+- Kecerdasan Buatan
+- Rekayasa Perangkat Lunak
+- Infrastruktur &amp; Security
+Profil Lulusan
+System Analyst, Software Engineer, Application Developer, DevOps Engineer, IT Security, Product Software Manager, Game Developer, Data Communication Engineer, Network Engineer, UX Researcher, UI/UX Designer, dan sebagainya.</t>
+  </si>
+  <si>
+    <t>Program sarjana studi Ilmu Komputer Fasilkom UI</t>
+  </si>
+  <si>
+    <t>PROGRAM SARJANA
+Program Studi Sistem Informasi
+cs.ui.ac.id/ssi
+GELAR
+Sarjana Ilmu Komputer (S. Kom)
+LOKASI KAMPUS
+Kampus UI Depok
+JADWAL PERKULIAHAN
+Pagi/Hari Kerja
+LAMA STUDI
+8 Semester (144 SKS)
+BAHASA
+Indonesia
+AKREDITASI
+A
+Program Studi Sarjana Sistem Informasi terdiri dari program reguler dan program non reguler. Program ini dirancang untuk memenuhi kebutuhan terhadap tenaga-tenaga yang terampil dan profesional di bidang sistem informasi/teknologi informasi. Program Studi Sistem Informasi mengajarkan landasan ilmu pengetahuan dan penerapan Teknologi Informasi dalam suatu organisasi. Terkait hal tersebut, kurikulum Program Studi Sistem Informasi bersifat unik karena menekankan keseimbangan antara kemampuan manajemen dan bisnis serta rekayasa informasi dan teknologi informasi.
+Kuliah-kuliah dasar membekali mahasiswa dengan kemampuan untuk merancang dan menulis program, terutama diarahkan untuk pengembangan Sistem Informasi dalam skala besar. Selain itu, mahasiswa juga akan mempelajari komponen-komponen dari Sistem Informasi/Teknologi Informasi, mulai dari sistem operasi, jaringan komputer, basis data, maupun aplikasi. 
+Untuk mengasah pemahaman di bidang bisnis dan manajemen, mahasiswa mempelajari konsep-konsep manajemen serta berbagai bisnis penunjang kegiatan organisasi dan dukungan yang bisa diberikan oleh Teknologi Informasi. Selain mata kuliah dasar, program studi sistem informasi juga menawarkan mata kuliah peminatan yang dikelompokkan ke dalam dua bidang minat berikut, yaitu:
+1. Solusi SI/TI
+2. E-Bisnis
+Profil Lulusan
+Sebagian besar lulusan Fasilkom UI bekerja di dalam maupun luar negeri di berbagai perusahaan nasional dan multinasional yang bergerak di bidang konsultan TI, asuransi, perbankan, telekomunikasi, industri perangkat lunak dan jasa, dan sebagainya. Beberapa posisi yang ditempati antara lain: system analyst, business analyst, IT manager, IT consultant, peneliti, IT auditor, data engineer system integrator, web developer, technical support, network administrator.</t>
+  </si>
+  <si>
+    <t>Program sarjana studi Sistem Informasi Fasilkom UI</t>
+  </si>
+  <si>
+    <t>International Undergraduate Program in Computer Science/Information Technology Fasilkom UI</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL UNDERGRADUATE PROGRAM
+in Computer Science/Information Technology (Double Degree)
+Mengapa Ilmu Komputer dan Teknologi Informasi (TI)?
+- Ilmu Komputer dan TI memenuhi kehidupan kita sehari-hari, setiap sektor bisnis, dan akan memainkan peran yang lebih penting di masa depan.
+- Kebutuhan profesional Ilmu Komputer dan IT di pasar kerja lokal, regional, dan internasional sangat tinggi.
+Sejak tahun 2002, Fakultas Ilmu Komputer Universitas Indonesia (Fasilkom UI) menjalin kerjasama dengan beberapa universitas rekanan untuk menawarkan Program Sarjana Internasional di bidang Ilmu Komputer/Teknologi Informasi. Program ini mempersiapkan mahasiswanya untuk menjadi lulusan yang mampu mengatasi tantangan di era globalisasi, bersaing di pasar kerja regional dan internasional, serta mampu mengejar gelar yang lebih tinggi. Program ini dijalankan oleh dosen yang berkualitas dan berpengalaman di bidang Ilmu Komputer dan Teknologi Informasi dari institusi terkait.
+cs.ui.ac.id/sik-kki
+GELAR
+Sarjana Ilmu Komputer (S. Kom) &amp; Bachelor of Information Technology, Bachelor of Computer Science, or Bachelor of Advanced Computing (Honours)
+LOKASI KAMPUS
+Kampus UI Depok (4-5 Semester)
+Australia dan UK (3-4 Semester)
+JADWAL PERKULIAHAN
+Pagi/Hari Kerja
+BAHASA
+Inggris
+AKREDITASI
+A
+- Bidang-bidang ini berkembang pesat dengan peluang menarik dalam mendorong batas-batas sains dan teknologi.
+- Ilmu Komputer dan IT saat ini juga mendukung kreativitas dan hiburan, mulai dari jejaring sosial hingga desain game.
+Mengapa Program Ini?
+Keunggulan program ini:
+- Pendidikan berkualitas tinggi dari universitas terkemuka di Indonesia dan luar negeri.
+- Sebagai mahasiswa kelas internasional, akan memiliki kesempatan untuk menjadi bagian dari program menarik ini dengan rekam jejak yang terbukti, yang memungkinkan memperoleh dua gelar Sarjana: Sarjana Ilmu Komputer (S.Kom.) Dari UI dan Sarjana Teknologi Informasi atau Sarjana Ilmu Komputer dari universitas rekanan. Untuk ANU, Bachelor of Advanced Computing (Honours) akan diberikan. Untuk University of Birmingham, mahasiswa dapat memilih B.Sc. Ilmu Komputer atau B.Sc. Kecerdasan Buatan dan Ilmu Komputer.
+- Biaya studi lebih rendah dibandingkan mengambil studi sarjana penuh waktu di universitas rekanan di luar negeri.
+- Semua mata kuliah yang ditawarkan di Fasilkom UI dan universitas rekanan, disampaikan dalam bahasa Inggris.
+- Perkuliahan dilakukan di kelas kecil.
+Lama Studi
+Program 4 tahun (8 semester). Bergantung pada gelar yang ditawarkan oleh universitas rekanan, program ini diatur sebagai
+- Skema 2.5 + 1.5, yaitu semester 1 - 5 di Fasilkom UI dan semester 6 - 8 di universitas rekanan (UQ* dan RMIT).
+- Skema 2 + 2 yaitu semester 1 - 4 di Fasilkom UI dan semester 5 - 8 di universitas rekanan (ANU, Deakin atau Univ. Birmingham) *) Bergantung pada jurusan yang ditawarkan oleh UQ, variasi skema 2.5 + 2 mungkin berlaku.
+Universitas Rekanan
+- The School of Information Technology and Electrical Engineering at the University of Queensland (UQ).
+- The College of Engineering &amp; Computer Science at the Australian National University (ANU).
+- The School of Information Technology at Deakin University.
+- The School of Computer Science at University of Birmingham, United Kingdom.
+- Royal Melbourne Institute of Technology (RMIT)
+Bidang Minat
+Peminatan yang ditawarkan dalam program ini mencakup bidang-bidang termasuk (tetapi tidak terbatas pada):
+- Kecerdasan buatan
+- Sistem dan Arsitektur
+- Ilmu Komputer Teoritis
+- Keamanan cyber
+- Ilmu Data
+- Komputasi Ilmiah
+- Sistem Informasi Perusahaan
+- Rekayasa Perangkat Lunak
+- Desain Pengalaman Pengguna
+- Pengembangan Game
+- Realitas Virtual dan Augmented</t>
+  </si>
+  <si>
+    <t>PROGRAM PASCASARJANA
+Magister Ilmu Komputer
+Program Studi Magister Ilmu Komputer (MIK) dibuka pada tahun 1988 dan dirancang untuk menghasilkan lulusan dengan wawasan riset dalam bidang ilmu komputer sebagai kelanjutan dari jenjang Sarjana bidang Ilmu Komputer. MIK menekankan integrasi antara pendidikan magister dan kegiatan penelitian. Mahasiswa diharapkan terlibat aktif dalam penelitian di Fakultas Ilmu Komputer UI. Kurikulum MIK disusun sedemikian rupa sehingga mahasiswa mendapatkan kesempatan untuk memperoleh pengetahuan yang luas dan pengalaman penelitian dalam bidang Ilmu Komputer. Pilihan-pilihan mata kuliah diberikan supaya mahasiswa dapat menyusun program pendidikannya sesuai dengan minat penelitiannya.
+GELAR
+Magister Ilmu Komputer (M.Kom)
+LOKASI KAMPUS
+Kampus UI Depok
+JADWAL PERKULIAHAN
+Pagi-Siang/Hari Kerja
+LAMA STUDI
+4 Semester
+BAHASA
+Indonesia
+AKREDITASI
+Unggul dari Lembaga Akreditasi Mandiri Informatika dan Komputer (LAM INFOKOM)
+cs.ui.ac.id/mik
+Ujian Penempatan
+Setelah diterima di program MIK, setiap mahasiswa baru harus mengambil sebuah Ujian Penempatan (Placement Test) yang mengevaluasi kemampuan serta pengetahuan mahasiswa untuk dikelompokan ke dalam salah satu dari dua (2) bidang peminatan: Ilmu komputer dan sistem informasi.
+Kurikulum
+Seiring perkembangan penelitian, kapasitas sumber daya manusia, cakupan penelitian tesis yang dikerjakan mahasiswa, serta memerhatikan perkembangan bidang Ilmu Komputer. Terdapat ujian bidang minat sebelum perkuliahan semester satu dimulai. Ujian ini dijadikan dasar dalam penentuan bidang minat mahasiswa. Mahasiswa diharapkan mampu mengembangkan bidang keilmuan dari masing-masing bidang minat yang dipilih.
+Profil Lulusan
+Sebagian besar lulusan Fasilkom UI bekerja di dalam maupun luar negeri di berbagai perusahaan nasional dan multinasional yang bergerak di bidang konsultasi teknologi informasi, perbankan, industri perangkat lunak dan jasa lainnya. Sebagian lainnya bekerja di institusi pemerintahan/perguruan tinggi, atau meneruskan pendidikan ke jenjang yang lebih tinggi di dalam dan luar negeri. Di samping itu, beberapa lulusan terjun langsung membangun perusahaan-perusahaan start-up.</t>
+  </si>
+  <si>
+    <t>Program Pascasarjana Magister Ilmu Komputer Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Program Pascasarjana Magister Teknologi Informasi Fasilkom UI</t>
+  </si>
+  <si>
+    <t>PROGRAM PASCASARJANA
+Magister Teknologi Informasi
+GELAR
+Magister Teknologi Informasi (M.T.I.)
+LOKASI KAMPUS
+Kampus UI Salemba
+JADWAL PERKULIAHAN
+- Kelas malam: setiap Senin-Jumat pukul 19:00 - 21:30 WIB.
+- Kelas siang: pukul 14:00 - 16:30 WIB. Namun kelas siang hanya dibuka apabila jumlah peserta mencukupi.
+LAMA STUDI
+4 Semester
+BAHASA
+Indonesia
+AKREDITASI
+A
+cs.ui.ac.id/mti
+Dalam dekade terakhir, bidang Teknologi Informasi (TI) telah berkembang sangat pesat. Peranan TI menjadi urat nadi organisasi modern dalam melakukan operasi dan manajemen bisnis. Secara khusus, kecenderungan ini melahirkan suatu kebutuhan akan sumber daya manusia untuk membangun dan mengelola TI. Program Magister Teknologi Informasi (SK DIKTI No. 2006/D/T/2005 tanggal 24 Juni 2005) di bawah naungan Fakultas Ilmu Komputer Universitas Indonesia (Fasilkom UI) dirancang untuk mengisi kesenjangan dari kebutuhan dunia industri dan bisnis untuk tenaga profesional, dengan keahlian dalam bidang TI.
+Karakteristik Program Magister Teknologi Informasi (MTI) ini antara lain:
+- Penekanan pada kemampuan integrasi yang kuat antara penerapan TI dan pengetahuan yang dalam mengenai manajemen serta strategi organisasi.
+- Berkembangnya berbagai karakteristik keahlian dalam bidang TI yang perlu pengajian lebih mendalam yang terkait dengan berbagai sektor bisnis dan industri.
+Kompetensi dan kemampuan yang menjadi sasaran program MTI-Fasilkom UI adalah:
+1. Intisari pengetahuan dan keahlian dalam bidang TI.
+2. Integrasi TI dalam fungsi dan dasar bisnis/organisasi serta dukungan pada karir.
+3. Kemampuan komunikasi, interpersonal dan bekerja dalam tim pada lingkup bisnis/organisasi.
+Untuk mendukung proses penelitiannya, program MTI ini didukung oleh Lab dengan kajian berbasis Teknologi Informasi yaitu Lab E-Government &amp; E-Business dan Lab Information Management.
+Kurikulum dirancang untuk mendukung bidang pekerjaan dalam lingkup manajemen TI (seperti perencanaan TI/SI, penerapan TI, pengelolaan TI, pengembangan perangkat lunak, dan sebagainya) maupun kesempatan karir pada bidang yang relatif baru (seperti konsultasi dan integrasi sistem, infrastruktur jaringan, e-business, IT Governance, digital economy dan sebagainya). Persiapan karir (career tracks) didukung oleh kewajiban untuk pendalaman dan spesialisasi TI melalui Karya Akhir.
+Peminatan:
+- Enterprise Software Solutions
+- Strategic IT Applications
+- IS/IT Governance
+- Cyber Security
+- Business Analytics
+- Digital Economy
+Profil Lulusan:
+Lulusan MTI diharapkan mempunyai kemampuan dan kompetensi untuk menjembatani bidang TI dan bisnis/organisasi. Para lulusan mendapatkan nilai tambah berupa kemampuan penyelesaian masalah Sistem Informasi dan Teknologi Informasi berdasarkan kajian studi kasus bersama akademisi dan praktisi. Di samping itu, peserta mendapatkan keahlian dalam mengartikulasi masalah atau solusi teknis dalam lintas organisasi, maupun dengan bahasa bisnis.
+Program Gelar Ganda (Double Degree):
+Program ini diselenggarakan dengan skema: tahun pertama perkuliahan di MTI Fasilkom UI dan tahun kedua di universitas mitra di luar negeri. Mahasiswa akan memperoleh dua gelar (dari Fasilkom UI dan universitas rekanan).
+Universitas Rekanan:
+Melbourne School of Engineering at the University of Melbourne
+Title: Master of Information Systems</t>
+  </si>
+  <si>
+    <t>PROGRAM PASCASARJANA
+Magister Teknologi Informasi e-Government
+GELAR
+Magister Teknologi Informasi (M.T.I.)
+LOKASI KAMPUS
+Kampus UI Salemba
+JADWAL PERKULIAHAN
+Malam/Hari Kerja
+LAMA STUDI
+4 Semester
+BAHASA
+Indonesia
+AKREDITASI
+A
+Program Magister Teknologi Informasi (MTI) e-Government merupakan Program Beasiswa Dalam Negeri Kominfo, yang dilaksanakan dengan tujuan mewujudkan SDM aparatur pemerintah yang unggul dalam pengembangan e-Government di lingkungan instansi pemerintah Pusat dan Daerah sesuai dengan Instruksi Presiden No. 3 Tahun 2003 tentang Kebijakan dan Strategi Nasional Pengembangan e-Government. Sasaran program ini adalah tersedianya SDM pengelola e-Government di lingkungan instansi Pemerintah Pusat dan Daerah. Fakultas Ilmu Komputer Universitas Indonesia bekerjasama dengan Kementerian Komunikasi dan Informatika dalam penyelenggaraan Program Beasiswa Dalam Negeri Kominfo.
+Profil Lulusan
+Lulusan MTI-Fasilkom UI diharapkan memiliki kemampuan dan kompetensi untuk menjembatani bidang TI dan bisnis/organisasi. Para lulusan mendapatkan nilai tambah berupa kemampuan penyelesaian masalah Sistem Informasi dan Teknologi Informasi berdasarkan kajian studi kasus bersama akademisi dan praktisi. Di samping itu, peserta mendapatkan keahlian dalam mengartikulasi masalah atau solusi teknis dalam lintas organisasi, maupun dengan bahasa bisnis.</t>
+  </si>
+  <si>
+    <t>Program Pascasarjana Magister Teknologi e-Government Informasi Fasilkom UI</t>
+  </si>
+  <si>
+    <t>PROGRAM PASCASARJANA
+Doktor Ilmu Komputer
+cs.ui.ac.id/dik
+GELAR
+Doktor (Dr.)
+LOKASI KAMPUS
+Kampus UI Depok
+JADWAL PERKULIAHAN
+Pagi/Hari Kerja
+LAMA STUDI
+6-10 Semester
+BAHASA
+Indonesia
+AKREDITASI
+Unggul dari Lembaga Akreditasi Mandiri Informatika dan Komputer (LAM INFOKOM)
+Program Studi Doktor Ilmu Komputer (DIK) yang dibuka pada tahun 1998 dirancang untuk mencetak lulusan yang memiliki kemampuan meneliti dalam bidang Ilmu Komputer sebagai kelanjutan jenjang magister bidang Ilmu Komputer.
+Program studi DIK menekankan integrasi antara pendidikan pascasarjana dan kegiatan riset. Mahasiswa diharapkan aktif dalam riset di Fakultas Ilmu Komputer UI. Kurikulum program studi DIK disusun sedemikian rupa sehingga mahasiswa mendapatkan kesempatan untuk memperoleh pengetahuan yang luas dan pengalaman meneliti dalam bidang Ilmu Komputer. Pilihan-pilihan mata ajar diberikan supaya mahasiswa dapat menyusun program pendidikannya sesuai dengan minat risetnya.
+Dari segi keilmuan dan keprofesian, lulusan dari program studi ini diharapkan mempunyai kompetensi utama sebagai berikut:
+- Mampu menciptakan orisinalitas/pembaruan dari perkembangan mutakhir state of the art di bidang ilmu komputer/komputasi.
+- Mampu menyusun artikel ilmiah dan dipublikasikan dalam jurnal berstandar internasional yang direview oleh pakar pada bidangnya.
+- Mampu merekomendasikan penyelesaian permasalahan kompleks di bidang ilmu komputasi melalui pendekatan inter, multi, dan transdisipliner.
+- Menunjukkan kedewasaan dalam berpikir terbuka dan tanggap terhadap perkembangan di bidang ilmu komputasi.
+- Mampu mengelola, memimpin, dan mengembangkan riset pada bidang ilmu komputer.
+Kurikulum
+Kurikulum Program Studi Doktor Ilmu Komputer (DIK) dirancang dan disusun sedemikian rupa sehingga para mahasiswa mendapatkan kesempatan untuk memperoleh pengetahuan yang luas dan pengalaman melakukan riset dalam bidang-bidang teknologi informasi dan komunikasi (TIK) seperti ilmu komputer, sistem informasi, rekayasa perangkat lunak, dan lain-lain. Kurikulum Program Studi DIK dirancang untuk diselesaikan dalam 6 semester, dan paling lama adalah 10 semester.
+Mata Kuliah
+Semester 1:
+- Metodologi Penelitian dan Penelitian Ilmiah
+- Filsafat: Ilmu, Metodologi &amp; Etika
+- Studi Mandiri 1/Kuliah Peminatan Lanjut
+Semester 2:
+- Studi Mandiri 2/Kuliah Peminatan Lanjut
+- Studi Mandiri 3/Kuliah Peminatan Lanjut
+- Ujian Proposal Riset
+Semester 3:
+- Ujian Hasil Riset
+- Makalah Ilmiah dan Sidang Pra Promosi
+Semester 4:
+- Sidang Promosi
+Profil Lulusan
+Dari segi keilmuan dan keprofesian, lulusan dari program studi ini diharapkan mempunyai karakteristik sebagai berikut:
+1. Terbuka dan tanggap terhadap perkembangan ilmu dan teknologi, khususnya yang menyangkut ilmu komputer.
+2. Mampu mengenali dan mengamati masalah-masalah di bidang Ilmu Komputer, serta melakukan pendekatan dan penalaran ilmiah untuk mencari pemecahannya.
+3. Mampu mengembangkan Ilmu Komputer lebih lanjut sehingga dapat mencapai derajat akademik yang lebih tinggi.</t>
+  </si>
+  <si>
+    <t>Program Pascasarjana Dokter Ilmu Komputer Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Here's the organized information about the research laboratories and centers at the Faculty of Computer Science, University of Indonesia:
+1. **Digital Library &amp; Distance Learning (DL2)**
+   - Head of Lab: Prof. Dr. Harry B. Santoso, Ph.D
+   - Website: dl2.cs.ui.ac.id
+   - Focus: Development of theory and information systems, particularly in e-learning and user experience (UX). Also, research extends to digital business, focusing on UX aspects.
+   - Recent Research Topics:
+     - Open Education Resources (OER)
+     - Massive Open Online Learning (MOOC)
+     - User Experience Design Measurements
+     - Digital Business User Experience
+2. **Machine Learning &amp; Computer Vision (MLCV)**
+   - Head of Lab: Dr. Ir. Erdefi Rakun, M.Sc.
+   - Website: mlcv.cs.ui.ac.id
+   - Focus: Research related to the manipulation, analysis, and interpretation of image data. Various methods are used, ranging from pixel-level processing to geometric division of images.
+   - Recent Research Topics:
+     - Feature Extraction and Selection (Color, Texture, Shape, Association Rules)
+     - Image Segmentation, Clustering, and Classification
+     - Object Matching and Recognition
+     - Content-Based Image Retrieval System (CBIR)
+3. **Intelligent Robots &amp; Systems (IRoS)**
+   - Head of Lab: Prof. Dr. Eng. Wisnu Jatmiko
+   - Focus: Primarily on Computer Networks, Computer Architecture, and High-Performance Computing. Aims to develop analytical abilities in computer architecture and design intelligent computer systems like robots.
+   - Recent Research Topics:
+     - Tele-USG and Tele-EKG
+     - Odor Source Localization with Swarm Robot
+     - Wireless Sensor Network
+     - Grid/High-Performance Computing to support drug design process
+4. **E-Government &amp; E-Business (EGB)**
+   - Head of Lab: Prof. Dana Indra Sensuse, Ph.D
+   - Website: egb.cs.ui.ac.id
+   - Focus: Combining expertise in technology (web services, network architecture, data engineering, business process modeling, and human-computer interaction) related to e-government and e-business development and integration.
+   - Recent Research Topics:
+     - e-Government and smart city
+     - Digital business
+     - Knowledge management
+     - IS/IT adoption
+5. **Information Management (IM)**
+   - Head of Lab: Dr. Muhammad Rifki Shihab, B.B.A., M.Sc.
+   - Website: im.cs.ui.ac.id
+   - Focus: Research in various areas of information retrieval such as Cross-language Information Retrieval (CLIR), Geographical Information Retrieval, Music Retrieval, and Image Retrieval.
+   - Recent Research Topics:
+     - Text mining
+     - Computational linguistics
+     - Natural language processing
+     - Information retrieval
+     - Plagiarism detection
+6. **Reliable Software Engineering (RSE)**
+   - Head of Lab: Prof. Eko K. Budiardjo, Ph.D
+   - Website: rse.cs.ui.ac.id
+   - Focus: Research on developing safe and reliable software from various aspects, such as requirements engineering, maintainability, testability, etc.
+   - Recent Research Topics:
+     - Software Product Line Engineering (SPLE)
+     - Theorem Prover
+     - Program Refinement
+     - Software Quality Assurance
+7. **Information Retrieval and Natural Language Processing (IRNLP)**
+   - Head of Lab: Prof. Dr. Indra Budi
+   - Website: ir.cs.ui.ac.id/new
+   - Focus: Exploration of methods and techniques for organizing, representing, storing, and retrieving textual and multimedia information (speech, images, and music).
+   - Recent Research Topics: 
+     - Various subfields including Text mining, Computational linguistics, Natural language processing, and Plagiarism detection
+8. **Tokopedia-UI AI Center of Excellence**
+   - Directors: Dr. Adila A. Krisnadhi &amp; Dr. Fariz Darari
+   - Website: tokopedia-ai.cs.ui.ac.id
+   - Focus: Collaborative research center where researchers from various labs work together, focusing on solving real-life problems using AI approaches.
+   - Recent Research Topics:
+     - AI in e-commerce
+     - AI in finance
+     - AI in education
+9. **Cyber Security &amp; Cryptography Center (CSCC)**
+   - Chair: Ir. Wahyu Catur Wibowo, M.Sc., Ph.D.
+   - Website: security.cs.ui.ac.id
+   - Focus: Research and education to address cybersecurity challenges through multidisciplinary research initiatives.
+   - Recent Research Topics:
+     - Blockchain-based calculation information systems
+     - Threat modeling
+     - Secure computing
+     - Large systems security
+10. **Computer Systems Lab (CSL)**
+    - Chair: Muhammad Hafizhuddin Hilman, Ph.D.
+    - Website: csl.cs.ui.ac.id
+    - Focus: Developing protocols, algorithms, and frameworks for Big Data Management, Computer Networks, High-Performance Computing, and Real-Time Systems.
+    - Recent Research Topics:
+      - Computer networks
+      - Cloud computing
+      - Big data infrastructure</t>
+  </si>
+  <si>
+    <t>Laboratorium dan Pusat Penelitian Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Persyaratan Jalur Masuk Fasilkom UI</t>
+  </si>
+  <si>
+    <t>**PERSYARATAN JALUR MASUK PROGRAM STUDI SARJANA REGULER**
+Program pendidikan jenjang sarjana yang menerima lulusan SMA/sederajat dengan batasan usia ijazah maksimal 3 tahun kelulusan pada saat pendaftaran.
+Jalur masuk seleksi nasional:
+- SNBT, yaitu Seleksi Bersama Masuk Perguruan Tinggi Negeri yang diselenggarakan oleh panitia nasional melalui jalur ujian tertulis.
+- SNBP, yaitu Seleksi berdasarkan evaluasi melalui nilai jalur rapor/undangan.
+- Olimpiade Sains, yaitu Seleksi berdasarkan jalur rapor/undangan dimana calon mahasiswa memiliki prestasi Juara dalam ajang Olimpiade Sains dalam bidang Komputer.
+**PROGRAM STUDI SARJANA NON REGULER**
+Program pendidikan jenjang sarjana yang menerima lulusan SMA/sederajat tanpa batasan usia ijazah.
+Jalur masuk seleksi mandiri:
+- SIMAK UI (Seleksi Masuk UI), yaitu jalur Seleksi yang diselenggarakan oleh UI serentak di kota besar di Indonesia melalui jalur ujian tertulis. Registrasi online: [https://penerimaan.ui.ac.id](https://penerimaan.ui.ac.id)
+- PPKB (Prestasi dan Pemerataan Kesempatan Belajar), yaitu Seleksi berdasarkan nilai jalur rapor/undangan.
+**PROGRAM KELAS KHUSUS INTERNASIONAL (KKI)**
+Program ini bekerja sama dengan universitas rekanan di luar negeri yang memberikan atmosfer internasional dengan pengantar kelas menggunakan Bahasa Inggris. Program studi kelas internasional (KKI) memiliki program Gelar Ganda (Double Degree), yaitu program yang memiliki kurikulum khusus dengan memberikan kesempatan mahasiswa untuk menempuh studi di fasilkom UI dan di Universitas rekanan di luar negeri dalam satu masa studi dengan memperoleh gelar sarjana UI dan Universitas Rekanan.
+Jalur masuk Program KKI:
+- SIMAK UI program KKI yaitu Seleksi jalur ujian tertulis khusus program KKI.
+- Talent Scouting, yaitu Seleksi berdasarkan evaluasi melalui jalur undangan/rapor untuk kelas internasional, dengan menggunakan undangan terbatas ke sekolah yang mendapatkan undangan dari UI.
+Persyaratan Pendaftaran Program KKI:
+- Menyelesaikan program sekolah menengah atas (SMA) atau sederajat dalam lima tahun terakhir (lulusan sekolah menengah atas yang menguasai sains dan matematika).
+- Memenuhi persyaratan bahasa Inggris dari Institutional TOEFL, disertifikasi oleh ETS (skor PBT 500 atau skor iBT 61 atau skor CBT 173) atau skor IELTS 5,5.
+- Lulus Ujian Masuk UI untuk Program Sarjana Kelas Internasional.
+- Informasi tentang pendaftaran dan penerimaan: [https://admission.ui.ac.id](https://admission.ui.ac.id)
+- Informasi untuk siswa internasional: [https://international.ui.ac.id](https://international.ui.ac.id)
+**PROGRAM STUDI MAGISTER ILMU KOMPUTER (MIK)**
+Persyaratan Akademik:
+1. Calon berijazah sarjana (S1) di bidang Ilmu Komputer, Informatika, Teknik Komputer, Teknik Elektro, Matematika, Fisika, atau ilmu komputasional lainnya.
+2. Lulus sarjana dengan Indeks Prestasi tidak kurang dari 3,00 (pada skala 4,0).
+3. Lulus ujian saringan di tingkat Universitas yang meliputi Tes Potensi Akademik (TPA) dan Bahasa Inggris.
+**PROGRAM GELAR GANDA MAGISTER ILMU KOMPUTER (MIK) (DOUBLE DEGREE)**
+Program ini diselenggarakan dengan skema: tahun pertama perkuliahan di universitas dalam negeri dan tahun kedua di universitas partner di luar negeri. Mahasiswa akan memperoleh dua gelar (dari Fasilkom UI dan Universitas rekanan).
+Mekanisme Pendaftaran Program Double Degree:
+Calon mahasiswa melakukan pendaftaran online SIMAK UI (Seleksi Masuk UI) dan memilih program Magister Fasilkom UI yang akan ditempuh (MIK). Panduan selengkapnya tentang pendaftaran dan jadwal penerimaan mahasiswa baru, tersedia pada website penerimaan UI. Pelaksanaan seleksi terdiri dari: Seleksi administrasi, Tes Potensi Akademik, Tes Bahasa Inggris.
+Setelah diterima dan lolos seleksi di program Magister Fasilkom UI, mahasiswa dapat mengajukan ke Ketua Program Studi untuk rencana program Magister-Double Degree ke universitas partner. Pendaftaran ke universitas rekanan dilakukan secara online sesuai informasi dan panduan pada website universitas rekanan dengan ketentuan IPK dan bahasa Inggris sesuai dengan standar masing-masing rekanan.
+**PROGRAM STUDI MAGISTER TEKNOLOGI INFORMASI (MTI)**
+Persyaratan Akademik:
+Calon mahasiswa harus memenuhi persyaratan sebagai berikut:
+1. Lulus program Strata 1/Diploma 4 dengan latar belakang keilmuan: Ilmu Komputer, Teknik Informatika, Sistem Informasi, Teknik Komputer, Teknik Elektro, atau bidang keilmuan selain tersebut di atas dengan pengalaman kerja minimal 2 tahun di bidang Teknologi Informasi.
+2. Nilai IPK minimal 3.00 pada skala 4,00.
+3. Peserta dengan latar belakang pendidikan non Teknologi Informasi(TI) dapat mendaftar dengan menunjukkan bukti pengalaman kerja di bidang TI minimal 2 tahun terakhir. Bukti tersebut berupa surat keterangan kerja dan surat rekomendasi atasannya, yang diunggah bersama ijazah di menu unggah dokumen di [https://penerimaan.ui.ac.id](https://penerimaan.ui.ac.id).
+4. Lulus ujian Seleksi Masuk UI (SIMAK UI)
+   - Pendaftaran SIMAK UI online pada [http://penerimaan.ui.ac.id](http://penerimaan.ui.ac.id)
+   - Ujian SIMAK UI meliputi Tes Potensi Akademik (TPA) dan Bahasa Inggris.
+**PROGRAM -
+ GELAR GANDA MAGISTER TEKNOLOGI INFORMASI (MTI) (DOUBLE DEGREE)**
+Persyaratan Akademik:
+1. Calon mahasiswa melakukan pendaftaran online SIMAK UI (Seleksi Masuk UI) di [https://penerimaan.ui.ac.id](https://penerimaan.ui.ac.id) dan memilih program Magister Fasilkom UI yang akan ditempuh (MTI). Panduan selengkapnya tentang pendaftaran dan jadwal penerimaan mahasiswa baru, tersedia pada website penerimaan UI. Pelaksanaan seleksi terdiri dari: Seleksi administrasi, Tes Potensi Akademik, dan Tes Bahasa Inggris.
+2. Setelah diterima dan lolos seleksi di program Magister Fasilkom UI, mahasiswa yang bersangkutan dapat mengajukan ke Ketua Program Studi untuk rencana program Double Degree ke universitas partner. Pendaftaran ke universitas rekanan dilakukan secara online sesuai informasi dan panduan pada Website universitas rekanan. Pelaksanaan seleksi terdiri dari: seleksi administrasi dan
+**Tata Cara Pendaftaran**
+- Peminat mendaftarkan diri secara online di [https://penerimaan.ui.ac.id/](https://penerimaan.ui.ac.id/) untuk pendaftaran Seleksi Masuk (SIMAK) Universitas Indonesia. Panduan lengkap pendaftaran tersedia pada halaman penerimaan UI.
+- Setelah dinyatakan LULUS pada seleksi penerimaan di UI, calon penerima beasiswa akan menjalani seleksi lanjutan di Kementerian Kominfo dengan mempertimbangkan aspek-aspek akademis maupun kelengkapan berkas-berkas pendaftaran.
+- Pendaftar program beasiswa internal Kominfo, permohonan diajukan langsung oleh PNS calon penerima beasiswa.
+- Peserta yang dinyatakan sebagai penerima beasiswa Kementerian Kominfo akan mendapatkan SK Kepala Badan Litbang SDM Kementerian Kominfo, kemudian menandatangani Surat Perjanjian di atas materai.
+- Berkas formulir dan kelengkapan persyaratan dikirimkan ke alamat surel Sekretariat MTI ([sekreakademikmti@cs.ui.ac.id](mailto:sekreakademikmti@cs.ui.ac.id)).
+**PROGRAM DOKTOR ILMU KOMPUTER**
+**Kriteria Penerimaan Mahasiswa DIK**
+- Memperoleh persetujuan calon dosen pembimbing.
+- Lulus ujian tertulis saringan masuk Universitas yang terdiri dari TPA dan bahasa Inggris.
+- Lulus Ujian tertulis bidang ilmu dan ujian wawancara di tingkat Fakultas.
+- Kesesuaian usulan topik riset dengan kegiatan lab riset di Fasilkom UI.
+- Track record penelitian dan latar belakang akademik yang terkait dengan arah riset.
+- Komitmen waktu dan biaya untuk menyelesaikan studi DIK dengan baik.
+**Persyaratan Akademik**
+- Memiliki ijazah Magister pada latar belakang sebidang (ilmu komputer/informatika, sistem informasi, teknik komputer) atau yang terkait dengan topik riset yang diusulkan, dengan Indeks Prestasi Kumulatif (IPK) minimal 3,00 (pada skala 4,00). Untuk pendaftar yang latar belakang pendidikan (Sarjana dan Magister tidak sebidang, harus mengikuti program matrikulasi terlebih dahulu selama satu atau dua semester (ditentukan oleh tim seleksi pada saat wawancara).
+- Calon mahasiswa sudah harus mendapatkan pernyataan tertulis kesediaan calon pembimbing (gunakan template terlampir) dari seorang dosen tetap Fasilkom UI yang telah bergelar Doktoral. Dalam rangka memberikan persetujuan ini, dosen yang bersangkutan dapat saja memberikan tugas mandiri untuk menguji kesesuaian dan kelayakan potensi riset calon mahasiswa, misalnya membuat rangkuman paper ilmiah, atau mempresentasikan suatu topik tertentu. Calon mahasiswa perlu menghubungi calon pembimbing jauh-jauh hari sebelum batas pendaftaran. Daftar dosen yang dapat membimbing mahasiswa DIK dapat dilihat pada halaman Staf Pengajar.
+**Persyaratan Administrasi**
+- Mengikuti prosedur sistem pendaftaran online yang berlaku di UI [https://penerimaan.ui.ac.id](https://penerimaan.ui.ac.id) dan mengunggah hasil scan dokumen-dokumen berikut pada website tersebut:
+  1. Ijazah magister dan ijazah sarjana yang telah disahkan
+  2. Transkrip akademik magister dan sarjana yang telah disahkan
+- Menyerahkan berkas tambahan dan sebaiknya sudah diserahkan pada saat ujian bidang dalam bentuk hardcopy (ke Sekretariat Akademik, Lt. 2, Gd. B, Kampus Depok Fasilkom UI) dan softcopy (via email ke [sekreakademik@cs.ui.ac.id](mailto:sekreakademik@cs.ui.ac.id)):
+  1. Ijazah magister dan ijazah sarjana yang telah dilegalisir.
+  2. Transkrip akademik magister dan sarjana yang telah dilegalisir.
+  3. Lembar Research Statement (2-3 halaman) yang berisi pernyataan minat dan motivasi riset.
+  4. Surat rekomendasi dari dua mantan dosen pembimbing atau atasan mengenai kemampuan akademik.
+  5. Surat izin dari atasan (apabila sedang bekerja).
+  6. CV lengkap yang memperlihatkan track record terkait dengan arah riset (template).
+  7. Surat pernyataan kesanggupan untuk memenuhi kewajiban pembiayaan kuliah atau pernyataan beasiswa bila mendapatkan beasiswa dari institusi.
+  8. Surat pernyataan kesediaan calon pembimbing dari salah satu dosen Fakultas Ilmu Komputer yang telah bergelar doktor (template).
+  9. Proposal penelitian doktoral.</t>
+  </si>
+  <si>
+    <t>Tata cara pendaftaran Fasilkom UI</t>
+  </si>
+  <si>
+    <t>**Beasiswa POMDA**
+Selain beasiswa universitas dan sponsor eksternal, mahasiswa juga berkesempatan mendapatkan beasiswa dari Persatuan Orang Tua Mahasiswa, Dosen, dan Alumni (POMDA), suatu lembaga resmi di lingkungan Fasilkom UI sebagai wadah bergabungnya orang tua mahasiswa, dosen, dan alumni dalam misi mendukung terwujudnya proses belajar mengajar yang sehat, berkeadilan, dan berkualitas. POMDA membantu mahasiswa yang kurang mampu dengan memberikan beasiswa dalam bentuk biaya pendidikan, biaya hidup, dan lain-lain.
+**Beasiswa Universitas**
+Beasiswa Universitas Indonesia disalurkan dalam bentuk Biaya Operasional Pendidikan-Berkeadilan (BOP-B) yang merupakan skema pemberian beasiswa berupa pengurangan besaran BOP dan besaran Uang Pangkal (UP). Mahasiswa dapat mengajukan permohonan BOP-B sebelum periode registrasi administrasi dimulai sesuai dengan jalur penerimaan di Universitas. Mahasiswa yang mengajukan BOP-B akan dievaluasi keadaan finansialnya berdasarkan penghasilan orang tua, jumlah tanggungan orang tua, aset yang dimiliki, dan rekomendasi dari RT/RW.
+**Beasiswa Sponsor**
+Mahasiswa Sarjana Reguler UI juga mendapat kesempatan untuk memperoleh beasiswa dari pihak luar seperti pemerintah, bank, dan perusahaan swasta lainnya. Beasiswa yang diberikan beragam sifat maupun durasinya. Ada beasiswa yang hanya memberikan uang saku per bulan selama setahun, dan ada pula beasiswa yang memberikan uang saku bulanan ditambah dengan tunjangan BOP sampai mahasiswa tersebut lulus. Setiap tahunnya, sekitar 250 mahasiswa Sarjana Reguler Fasilkom dari seluruh angkatan mendapat beasiswa dari berbagai sponsor.</t>
+  </si>
+  <si>
+    <t>Beasiswa Fasilkom UI</t>
+  </si>
+  <si>
+    <t>**Pusat Ilmu Komputer Universitas Indonesia (Pusilkom UI)**
+Website: [https://www.pusilkom.ui.ac.id](https://www.pusilkom.ui.ac.id)
+Pusat Ilmu Komputer Universitas Indonesia (Pusilkom UI) didirikan pada tahun 1972 dengan latar belakang pembentukan untuk mengembangkan kompetensi civitas akademika Universitas Indonesia di bidang ilmu komputer. Sejak pembentukannya, Pusilkom UI telah aktif dalam mengembangkan ilmu komputer baik di dunia akademis, pemerintahan, maupun di dunia bisnis/industri.
+**Layanan Pusilkom UI**
+Sebagai unit usaha akademis dengan dukungan civitas akademika Fasilkom UI yang memiliki kompetensi di bidang ilmu komputer yang tidak diragukan lagi, Pusilkom UI menawarkan berbagai layanan di bidang teknologi informasi kepada kalangan industri, bisnis, dan pemerintah di Indonesia. Layanan-layanan tersebut meliputi training, konsultasi, pemrosesan data, pengembangan sistem informasi, dan riset.</t>
+  </si>
+  <si>
+    <t>Layanan Fasilkom UI</t>
+  </si>
+  <si>
+    <t>**Fakultas Ilmu Komputer Universitas Indonesia (Fasilkom UI)** adalah tempat yang menantang orang-orang dengan rasa ingin tahu yang tinggi dan bersemangat untuk berimajinasi dan berkarya di bidang ilmu komputer dan sistem informasi.
+Fasilkom UI merupakan salah satu institusi pendidikan tinggi terbaik di dunia dalam bidang ilmu komputer dan sistem informasi. Dengan riset yang mutakhir, start-up inovatif, ambisi yang besar, pembelajaran yang hands-on, dan robot-robot pintar, Fasilkom UI tidak hanya membayangkan masa depan, tapi juga turut membuatnya.
+- 2.800+ mahasiswa
+  - Terbaik dari seluruh penjuru nusantara
+- 80+ dosen
+  - Lulusan perguruan tinggi top dunia
+- 6.000+ alumni
+  - Dengan jaringan yang tersebar di tujuh benua</t>
+  </si>
+  <si>
+    <t>What is Fasilkom UI (Fakultas Ilmu Komputer Universitas Indonesia)</t>
   </si>
 </sst>
 </file>
@@ -306,14 +809,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7924FDD-4938-4597-972A-A9B3FA87D0C8}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -658,7 +1156,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -666,7 +1164,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -674,23 +1172,23 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
+      <c r="A7" t="s">
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -698,106 +1196,234 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>30</v>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data and minor update
</commit_message>
<xml_diff>
--- a/RISTEK.xlsx
+++ b/RISTEK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan\OneDrive\Documents\GitHub\RistekGPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97CE318-EF46-4F65-B9C7-585969A4BEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC5001F-4CA9-432D-8D5B-C8C6DE0ACD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A966B3A5-28D0-4C85-A779-BF24F350CC49}"/>
+    <workbookView xWindow="2280" yWindow="980" windowWidth="14400" windowHeight="9100" xr2:uid="{A966B3A5-28D0-4C85-A779-BF24F350CC49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="85">
   <si>
     <t>title</t>
   </si>
@@ -59,16 +59,7 @@
 Enjoy personalized service tailored to your needs. We'll collaborate closely with you to ensure the solution we deliver meets your exact specifications.</t>
   </si>
   <si>
-    <t>How long has RISTEK Fasilkom UI been operating?</t>
-  </si>
-  <si>
     <t>Operating for 34 years, RISTEK Fasilkom UI is an independent organization within the Faculty of Computer Science at Universitas Indonesia. Its mission is to cultivate students’ interest and talent in technology, producing highly skilled individuals in various fields. Serving as the primary hub for students' innovation, RISTEK Fasilkom UI has developed over 40 products used by tens of thousands annually. The organization has also achieved success in both local and international competitions. Driven by values of excellence, synergy, and equity, RISTEK Fasilkom UI assists clients in fulfilling their digital aspirations by offering top talents from Universitas Indonesia for their software development needs.</t>
-  </si>
-  <si>
-    <t>How does RISTEK Fasilkom UI contribute to its clients' digital aspirations?</t>
-  </si>
-  <si>
-    <t>What is RISTEK Fasilkom UI</t>
   </si>
   <si>
     <t>We strive for excellence
@@ -77,30 +68,6 @@
 - Purposeful partnerships with external entities and effective collaboration across internal teams act as catalysts for us to achieve our mission.
 We aim to achieve equity
 - Along with the purpose to provide equal opportunities &amp; resources to each member, we are committed to support them to grow to their maximum potential.</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI Achievements</t>
-  </si>
-  <si>
-    <t>Benefits for RISTEK Fasilkom UI members</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI susun jadwal</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI Ulas Kelas</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI products</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI projects</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI contact</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI location</t>
   </si>
   <si>
     <t>Our members are a part of diverse divisions that work together as one.
@@ -140,9 +107,6 @@
 Product Operations
 About Us
 Product Operations (referred to as Product Ops) is a part of the Product Office team. As a member of Product Ops, you will be a part of an independent team directly under the Executive Director of Product.</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI ristek.link</t>
   </si>
   <si>
     <t>Here's a showcase of our past projects and capabilities:
@@ -258,9 +222,6 @@
 #1 Juara Umum GEMASTIK (GEMASTIK 2016-2020)</t>
   </si>
   <si>
-    <t>Fasilkom UI overall achievements</t>
-  </si>
-  <si>
     <t>Sejarah Fakultas Ilmu Komputer Universitas Indonesia (Fasilkom UI) adalah tempat yang menantang orang-orang dengan rasa ingin tahu yang tinggi dan bersemangat untuk berimajinasi dan berkarya di bidang ilmu komputer dan sistem informasi. Fasilkom UI merupakan salah satu institusi pendidikan tinggi terbaik di dunia dalam bidang ilmu komputer dan sistem informasi. Dengan riset yang mutakhir, start-up inovatif, ambisi yang besar, pembelajaran yang hands-on, dan robot-robot pintar, Fasilkom UI tidak hanya membayangkan masa depan, tapi juga turut membuatnya.
 1972 - Sejarah Fakultas Ilmu Komputer Universitas Indonesia tidak dapat dipisahkan dari pendirian Pusat Ilmu Komputer Universitas Indonesia (Pusilkom UI) pada tahun 1972.
 1986 - Berangkat dari desakan dari berbagai pihak kepada UI untuk menyelenggarakan program pendidikan ilmu komputer, maka pada tahun 1986 Pusilkom UI mulai menyelenggarakan program studi ilmu komputer untuk jenjang sarjana.
@@ -270,30 +231,6 @@
 1998 - Menjelang akhir milenium, Fasilkom UI memulai program doktor ilmu komputer pertama di Indonesia pada tahun 1998.
 2002 - Menanggapi permintaan akan talenta ilmu komputer dengan wawasan global, Fasilkom UI membuka program studi ilmu komputer kelas internasional.
 2007 - Seiring dengan meningkatnya peran ilmu komputer dalam konteks organisasi, Fasilkom UI membuka program studi Sistem Informasi dan Program Parelel Lanjutan D3 (Ekstensi) Sistem Informasi.</t>
-  </si>
-  <si>
-    <t>Sejarah Fasilkom UI</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI divisions</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI events</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI values</t>
-  </si>
-  <si>
-    <t>RISTEK Fasilkom UI services</t>
-  </si>
-  <si>
-    <t>Benefits to collaborate with RISTEK Fasilkom UI</t>
-  </si>
-  <si>
-    <t>Reason to Collaborate with RISTEK Fasilkom UI</t>
-  </si>
-  <si>
-    <t>Primary goal of RISTEK Fasilkom UI</t>
   </si>
   <si>
     <t>Visi
@@ -309,9 +246,6 @@
 Bertanggung jawab secara moral dan sosial pada pengembangan kecerdasan dan martabat bangsa.
 Budaya Organisasi
 Bersama membangun layanan prima, cerdas dan berkualitas dengan motto "Excellence in Teamwork". Fasilkom UI merancang kegiatan akademik yang terpadu antara Pendidikan, Penelitian &amp; Pelayanan, dan Program Penjangkauan. Segenap sumber daya dikerahkan untuk menunjang tiga aspek kegiatan akademik tersebut.</t>
-  </si>
-  <si>
-    <t>Visi dan Misi Fasilkom UI</t>
   </si>
   <si>
     <t>PROGRAM SARJANA
@@ -338,9 +272,6 @@
 System Analyst, Software Engineer, Application Developer, DevOps Engineer, IT Security, Product Software Manager, Game Developer, Data Communication Engineer, Network Engineer, UX Researcher, UI/UX Designer, dan sebagainya.</t>
   </si>
   <si>
-    <t>Program sarjana studi Ilmu Komputer Fasilkom UI</t>
-  </si>
-  <si>
     <t>PROGRAM SARJANA
 Program Studi Sistem Informasi
 cs.ui.ac.id/ssi
@@ -363,12 +294,6 @@
 2. E-Bisnis
 Profil Lulusan
 Sebagian besar lulusan Fasilkom UI bekerja di dalam maupun luar negeri di berbagai perusahaan nasional dan multinasional yang bergerak di bidang konsultan TI, asuransi, perbankan, telekomunikasi, industri perangkat lunak dan jasa, dan sebagainya. Beberapa posisi yang ditempati antara lain: system analyst, business analyst, IT manager, IT consultant, peneliti, IT auditor, data engineer system integrator, web developer, technical support, network administrator.</t>
-  </si>
-  <si>
-    <t>Program sarjana studi Sistem Informasi Fasilkom UI</t>
-  </si>
-  <si>
-    <t>International Undergraduate Program in Computer Science/Information Technology Fasilkom UI</t>
   </si>
   <si>
     <t>INTERNATIONAL UNDERGRADUATE PROGRAM
@@ -447,12 +372,6 @@
 Sebagian besar lulusan Fasilkom UI bekerja di dalam maupun luar negeri di berbagai perusahaan nasional dan multinasional yang bergerak di bidang konsultasi teknologi informasi, perbankan, industri perangkat lunak dan jasa lainnya. Sebagian lainnya bekerja di institusi pemerintahan/perguruan tinggi, atau meneruskan pendidikan ke jenjang yang lebih tinggi di dalam dan luar negeri. Di samping itu, beberapa lulusan terjun langsung membangun perusahaan-perusahaan start-up.</t>
   </si>
   <si>
-    <t>Program Pascasarjana Magister Ilmu Komputer Fasilkom UI</t>
-  </si>
-  <si>
-    <t>Program Pascasarjana Magister Teknologi Informasi Fasilkom UI</t>
-  </si>
-  <si>
     <t>PROGRAM PASCASARJANA
 Magister Teknologi Informasi
 GELAR
@@ -512,9 +431,6 @@
 Program Magister Teknologi Informasi (MTI) e-Government merupakan Program Beasiswa Dalam Negeri Kominfo, yang dilaksanakan dengan tujuan mewujudkan SDM aparatur pemerintah yang unggul dalam pengembangan e-Government di lingkungan instansi pemerintah Pusat dan Daerah sesuai dengan Instruksi Presiden No. 3 Tahun 2003 tentang Kebijakan dan Strategi Nasional Pengembangan e-Government. Sasaran program ini adalah tersedianya SDM pengelola e-Government di lingkungan instansi Pemerintah Pusat dan Daerah. Fakultas Ilmu Komputer Universitas Indonesia bekerjasama dengan Kementerian Komunikasi dan Informatika dalam penyelenggaraan Program Beasiswa Dalam Negeri Kominfo.
 Profil Lulusan
 Lulusan MTI-Fasilkom UI diharapkan memiliki kemampuan dan kompetensi untuk menjembatani bidang TI dan bisnis/organisasi. Para lulusan mendapatkan nilai tambah berupa kemampuan penyelesaian masalah Sistem Informasi dan Teknologi Informasi berdasarkan kajian studi kasus bersama akademisi dan praktisi. Di samping itu, peserta mendapatkan keahlian dalam mengartikulasi masalah atau solusi teknis dalam lintas organisasi, maupun dengan bahasa bisnis.</t>
-  </si>
-  <si>
-    <t>Program Pascasarjana Magister Teknologi e-Government Informasi Fasilkom UI</t>
   </si>
   <si>
     <t>PROGRAM PASCASARJANA
@@ -561,9 +477,6 @@
 1. Terbuka dan tanggap terhadap perkembangan ilmu dan teknologi, khususnya yang menyangkut ilmu komputer.
 2. Mampu mengenali dan mengamati masalah-masalah di bidang Ilmu Komputer, serta melakukan pendekatan dan penalaran ilmiah untuk mencari pemecahannya.
 3. Mampu mengembangkan Ilmu Komputer lebih lanjut sehingga dapat mencapai derajat akademik yang lebih tinggi.</t>
-  </si>
-  <si>
-    <t>Program Pascasarjana Dokter Ilmu Komputer Fasilkom UI</t>
   </si>
   <si>
     <t>Here's the organized information about the research laboratories and centers at the Faculty of Computer Science, University of Indonesia:
@@ -654,10 +567,41 @@
       - Big data infrastructure</t>
   </si>
   <si>
-    <t>Laboratorium dan Pusat Penelitian Fasilkom UI</t>
-  </si>
-  <si>
-    <t>Persyaratan Jalur Masuk Fasilkom UI</t>
+    <t>**Beasiswa POMDA**
+Selain beasiswa universitas dan sponsor eksternal, mahasiswa juga berkesempatan mendapatkan beasiswa dari Persatuan Orang Tua Mahasiswa, Dosen, dan Alumni (POMDA), suatu lembaga resmi di lingkungan Fasilkom UI sebagai wadah bergabungnya orang tua mahasiswa, dosen, dan alumni dalam misi mendukung terwujudnya proses belajar mengajar yang sehat, berkeadilan, dan berkualitas. POMDA membantu mahasiswa yang kurang mampu dengan memberikan beasiswa dalam bentuk biaya pendidikan, biaya hidup, dan lain-lain.
+**Beasiswa Universitas**
+Beasiswa Universitas Indonesia disalurkan dalam bentuk Biaya Operasional Pendidikan-Berkeadilan (BOP-B) yang merupakan skema pemberian beasiswa berupa pengurangan besaran BOP dan besaran Uang Pangkal (UP). Mahasiswa dapat mengajukan permohonan BOP-B sebelum periode registrasi administrasi dimulai sesuai dengan jalur penerimaan di Universitas. Mahasiswa yang mengajukan BOP-B akan dievaluasi keadaan finansialnya berdasarkan penghasilan orang tua, jumlah tanggungan orang tua, aset yang dimiliki, dan rekomendasi dari RT/RW.
+**Beasiswa Sponsor**
+Mahasiswa Sarjana Reguler UI juga mendapat kesempatan untuk memperoleh beasiswa dari pihak luar seperti pemerintah, bank, dan perusahaan swasta lainnya. Beasiswa yang diberikan beragam sifat maupun durasinya. Ada beasiswa yang hanya memberikan uang saku per bulan selama setahun, dan ada pula beasiswa yang memberikan uang saku bulanan ditambah dengan tunjangan BOP sampai mahasiswa tersebut lulus. Setiap tahunnya, sekitar 250 mahasiswa Sarjana Reguler Fasilkom dari seluruh angkatan mendapat beasiswa dari berbagai sponsor.</t>
+  </si>
+  <si>
+    <t>Beasiswa Fasilkom UI</t>
+  </si>
+  <si>
+    <t>**Pusat Ilmu Komputer Universitas Indonesia (Pusilkom UI)**
+Website: [https://www.pusilkom.ui.ac.id](https://www.pusilkom.ui.ac.id)
+Pusat Ilmu Komputer Universitas Indonesia (Pusilkom UI) didirikan pada tahun 1972 dengan latar belakang pembentukan untuk mengembangkan kompetensi civitas akademika Universitas Indonesia di bidang ilmu komputer. Sejak pembentukannya, Pusilkom UI telah aktif dalam mengembangkan ilmu komputer baik di dunia akademis, pemerintahan, maupun di dunia bisnis/industri.
+**Layanan Pusilkom UI**
+Sebagai unit usaha akademis dengan dukungan civitas akademika Fasilkom UI yang memiliki kompetensi di bidang ilmu komputer yang tidak diragukan lagi, Pusilkom UI menawarkan berbagai layanan di bidang teknologi informasi kepada kalangan industri, bisnis, dan pemerintah di Indonesia. Layanan-layanan tersebut meliputi training, konsultasi, pemrosesan data, pengembangan sistem informasi, dan riset.</t>
+  </si>
+  <si>
+    <t>**Fakultas Ilmu Komputer Universitas Indonesia (Fasilkom UI)** adalah tempat yang menantang orang-orang dengan rasa ingin tahu yang tinggi dan bersemangat untuk berimajinasi dan berkarya di bidang ilmu komputer dan sistem informasi.
+Fasilkom UI merupakan salah satu institusi pendidikan tinggi terbaik di dunia dalam bidang ilmu komputer dan sistem informasi. Dengan riset yang mutakhir, start-up inovatif, ambisi yang besar, pembelajaran yang hands-on, dan robot-robot pintar, Fasilkom UI tidak hanya membayangkan masa depan, tapi juga turut membuatnya.
+- 2.800+ mahasiswa
+  - Terbaik dari seluruh penjuru nusantara
+- 80+ dosen
+  - Lulusan perguruan tinggi top dunia
+- 6.000+ alumni
+  - Dengan jaringan yang tersebar di tujuh benua</t>
+  </si>
+  <si>
+    <t>How long has RISTEK been operating?</t>
+  </si>
+  <si>
+    <t>How does RISTEK contribute to its clients' digital aspirations?</t>
+  </si>
+  <si>
+    <t>What is RISTEK</t>
   </si>
   <si>
     <t>**PERSYARATAN JALUR MASUK PROGRAM STUDI SARJANA REGULER**
@@ -665,13 +609,17 @@
 Jalur masuk seleksi nasional:
 - SNBT, yaitu Seleksi Bersama Masuk Perguruan Tinggi Negeri yang diselenggarakan oleh panitia nasional melalui jalur ujian tertulis.
 - SNBP, yaitu Seleksi berdasarkan evaluasi melalui nilai jalur rapor/undangan.
-- Olimpiade Sains, yaitu Seleksi berdasarkan jalur rapor/undangan dimana calon mahasiswa memiliki prestasi Juara dalam ajang Olimpiade Sains dalam bidang Komputer.
-**PROGRAM STUDI SARJANA NON REGULER**
+- Olimpiade Sains, yaitu Seleksi berdasarkan jalur rapor/undangan dimana calon mahasiswa memiliki prestasi Juara dalam ajang Olimpiade Sains dalam bidang Komputer.</t>
+  </si>
+  <si>
+    <t>**PROGRAM STUDI SARJANA NON REGULER**
 Program pendidikan jenjang sarjana yang menerima lulusan SMA/sederajat tanpa batasan usia ijazah.
 Jalur masuk seleksi mandiri:
 - SIMAK UI (Seleksi Masuk UI), yaitu jalur Seleksi yang diselenggarakan oleh UI serentak di kota besar di Indonesia melalui jalur ujian tertulis. Registrasi online: [https://penerimaan.ui.ac.id](https://penerimaan.ui.ac.id)
-- PPKB (Prestasi dan Pemerataan Kesempatan Belajar), yaitu Seleksi berdasarkan nilai jalur rapor/undangan.
-**PROGRAM KELAS KHUSUS INTERNASIONAL (KKI)**
+- PPKB (Prestasi dan Pemerataan Kesempatan Belajar), yaitu Seleksi berdasarkan nilai jalur rapor/undangan.</t>
+  </si>
+  <si>
+    <t>**PROGRAM KELAS KHUSUS INTERNASIONAL (KKI)**
 Program ini bekerja sama dengan universitas rekanan di luar negeri yang memberikan atmosfer internasional dengan pengantar kelas menggunakan Bahasa Inggris. Program studi kelas internasional (KKI) memiliki program Gelar Ganda (Double Degree), yaitu program yang memiliki kurikulum khusus dengan memberikan kesempatan mahasiswa untuk menempuh studi di fasilkom UI dan di Universitas rekanan di luar negeri dalam satu masa studi dengan memperoleh gelar sarjana UI dan Universitas Rekanan.
 Jalur masuk Program KKI:
 - SIMAK UI program KKI yaitu Seleksi jalur ujian tertulis khusus program KKI.
@@ -681,18 +629,24 @@
 - Memenuhi persyaratan bahasa Inggris dari Institutional TOEFL, disertifikasi oleh ETS (skor PBT 500 atau skor iBT 61 atau skor CBT 173) atau skor IELTS 5,5.
 - Lulus Ujian Masuk UI untuk Program Sarjana Kelas Internasional.
 - Informasi tentang pendaftaran dan penerimaan: [https://admission.ui.ac.id](https://admission.ui.ac.id)
-- Informasi untuk siswa internasional: [https://international.ui.ac.id](https://international.ui.ac.id)
-**PROGRAM STUDI MAGISTER ILMU KOMPUTER (MIK)**
+- Informasi untuk siswa internasional: [https://international.ui.ac.id](https://international.ui.ac.id)</t>
+  </si>
+  <si>
+    <t>**PROGRAM STUDI MAGISTER ILMU KOMPUTER (MIK)**
 Persyaratan Akademik:
 1. Calon berijazah sarjana (S1) di bidang Ilmu Komputer, Informatika, Teknik Komputer, Teknik Elektro, Matematika, Fisika, atau ilmu komputasional lainnya.
 2. Lulus sarjana dengan Indeks Prestasi tidak kurang dari 3,00 (pada skala 4,0).
-3. Lulus ujian saringan di tingkat Universitas yang meliputi Tes Potensi Akademik (TPA) dan Bahasa Inggris.
-**PROGRAM GELAR GANDA MAGISTER ILMU KOMPUTER (MIK) (DOUBLE DEGREE)**
+3. Lulus ujian saringan di tingkat Universitas yang meliputi Tes Potensi Akademik (TPA) dan Bahasa Inggris.</t>
+  </si>
+  <si>
+    <t>**PROGRAM GELAR GANDA MAGISTER ILMU KOMPUTER (MIK) (DOUBLE DEGREE)**
 Program ini diselenggarakan dengan skema: tahun pertama perkuliahan di universitas dalam negeri dan tahun kedua di universitas partner di luar negeri. Mahasiswa akan memperoleh dua gelar (dari Fasilkom UI dan Universitas rekanan).
 Mekanisme Pendaftaran Program Double Degree:
 Calon mahasiswa melakukan pendaftaran online SIMAK UI (Seleksi Masuk UI) dan memilih program Magister Fasilkom UI yang akan ditempuh (MIK). Panduan selengkapnya tentang pendaftaran dan jadwal penerimaan mahasiswa baru, tersedia pada website penerimaan UI. Pelaksanaan seleksi terdiri dari: Seleksi administrasi, Tes Potensi Akademik, Tes Bahasa Inggris.
-Setelah diterima dan lolos seleksi di program Magister Fasilkom UI, mahasiswa dapat mengajukan ke Ketua Program Studi untuk rencana program Magister-Double Degree ke universitas partner. Pendaftaran ke universitas rekanan dilakukan secara online sesuai informasi dan panduan pada website universitas rekanan dengan ketentuan IPK dan bahasa Inggris sesuai dengan standar masing-masing rekanan.
-**PROGRAM STUDI MAGISTER TEKNOLOGI INFORMASI (MTI)**
+Setelah diterima dan lolos seleksi di program Magister Fasilkom UI, mahasiswa dapat mengajukan ke Ketua Program Studi untuk rencana program Magister-Double Degree ke universitas partner. Pendaftaran ke universitas rekanan dilakukan secara online sesuai informasi dan panduan pada website universitas rekanan dengan ketentuan IPK dan bahasa Inggris sesuai dengan standar masing-masing rekanan.</t>
+  </si>
+  <si>
+    <t>**PROGRAM STUDI MAGISTER TEKNOLOGI INFORMASI (MTI)**
 Persyaratan Akademik:
 Calon mahasiswa harus memenuhi persyaratan sebagai berikut:
 1. Lulus program Strata 1/Diploma 4 dengan latar belakang keilmuan: Ilmu Komputer, Teknik Informatika, Sistem Informasi, Teknik Komputer, Teknik Elektro, atau bidang keilmuan selain tersebut di atas dengan pengalaman kerja minimal 2 tahun di bidang Teknologi Informasi.
@@ -700,9 +654,10 @@
 3. Peserta dengan latar belakang pendidikan non Teknologi Informasi(TI) dapat mendaftar dengan menunjukkan bukti pengalaman kerja di bidang TI minimal 2 tahun terakhir. Bukti tersebut berupa surat keterangan kerja dan surat rekomendasi atasannya, yang diunggah bersama ijazah di menu unggah dokumen di [https://penerimaan.ui.ac.id](https://penerimaan.ui.ac.id).
 4. Lulus ujian Seleksi Masuk UI (SIMAK UI)
    - Pendaftaran SIMAK UI online pada [http://penerimaan.ui.ac.id](http://penerimaan.ui.ac.id)
-   - Ujian SIMAK UI meliputi Tes Potensi Akademik (TPA) dan Bahasa Inggris.
-**PROGRAM -
- GELAR GANDA MAGISTER TEKNOLOGI INFORMASI (MTI) (DOUBLE DEGREE)**
+   - Ujian SIMAK UI meliputi Tes Potensi Akademik (TPA) dan Bahasa Inggris.</t>
+  </si>
+  <si>
+    <t>**PROGRAM - GELAR GANDA MAGISTER TEKNOLOGI INFORMASI (MTI) (DOUBLE DEGREE)**
 Persyaratan Akademik:
 1. Calon mahasiswa melakukan pendaftaran online SIMAK UI (Seleksi Masuk UI) di [https://penerimaan.ui.ac.id](https://penerimaan.ui.ac.id) dan memilih program Magister Fasilkom UI yang akan ditempuh (MTI). Panduan selengkapnya tentang pendaftaran dan jadwal penerimaan mahasiswa baru, tersedia pada website penerimaan UI. Pelaksanaan seleksi terdiri dari: Seleksi administrasi, Tes Potensi Akademik, dan Tes Bahasa Inggris.
 2. Setelah diterima dan lolos seleksi di program Magister Fasilkom UI, mahasiswa yang bersangkutan dapat mengajukan ke Ketua Program Studi untuk rencana program Double Degree ke universitas partner. Pendaftaran ke universitas rekanan dilakukan secara online sesuai informasi dan panduan pada Website universitas rekanan. Pelaksanaan seleksi terdiri dari: seleksi administrasi dan
@@ -711,8 +666,10 @@
 - Setelah dinyatakan LULUS pada seleksi penerimaan di UI, calon penerima beasiswa akan menjalani seleksi lanjutan di Kementerian Kominfo dengan mempertimbangkan aspek-aspek akademis maupun kelengkapan berkas-berkas pendaftaran.
 - Pendaftar program beasiswa internal Kominfo, permohonan diajukan langsung oleh PNS calon penerima beasiswa.
 - Peserta yang dinyatakan sebagai penerima beasiswa Kementerian Kominfo akan mendapatkan SK Kepala Badan Litbang SDM Kementerian Kominfo, kemudian menandatangani Surat Perjanjian di atas materai.
-- Berkas formulir dan kelengkapan persyaratan dikirimkan ke alamat surel Sekretariat MTI ([sekreakademikmti@cs.ui.ac.id](mailto:sekreakademikmti@cs.ui.ac.id)).
-**PROGRAM DOKTOR ILMU KOMPUTER**
+- Berkas formulir dan kelengkapan persyaratan dikirimkan ke alamat surel Sekretariat MTI ([sekreakademikmti@cs.ui.ac.id](mailto:sekreakademikmti@cs.ui.ac.id)).</t>
+  </si>
+  <si>
+    <t>**PROGRAM DOKTOR ILMU KOMPUTER**
 **Kriteria Penerimaan Mahasiswa DIK**
 - Memperoleh persetujuan calon dosen pembimbing.
 - Lulus ujian tertulis saringan masuk Universitas yang terdiri dari TPA dan bahasa Inggris.
@@ -739,41 +696,145 @@
   9. Proposal penelitian doktoral.</t>
   </si>
   <si>
-    <t>Tata cara pendaftaran Fasilkom UI</t>
-  </si>
-  <si>
-    <t>**Beasiswa POMDA**
-Selain beasiswa universitas dan sponsor eksternal, mahasiswa juga berkesempatan mendapatkan beasiswa dari Persatuan Orang Tua Mahasiswa, Dosen, dan Alumni (POMDA), suatu lembaga resmi di lingkungan Fasilkom UI sebagai wadah bergabungnya orang tua mahasiswa, dosen, dan alumni dalam misi mendukung terwujudnya proses belajar mengajar yang sehat, berkeadilan, dan berkualitas. POMDA membantu mahasiswa yang kurang mampu dengan memberikan beasiswa dalam bentuk biaya pendidikan, biaya hidup, dan lain-lain.
-**Beasiswa Universitas**
-Beasiswa Universitas Indonesia disalurkan dalam bentuk Biaya Operasional Pendidikan-Berkeadilan (BOP-B) yang merupakan skema pemberian beasiswa berupa pengurangan besaran BOP dan besaran Uang Pangkal (UP). Mahasiswa dapat mengajukan permohonan BOP-B sebelum periode registrasi administrasi dimulai sesuai dengan jalur penerimaan di Universitas. Mahasiswa yang mengajukan BOP-B akan dievaluasi keadaan finansialnya berdasarkan penghasilan orang tua, jumlah tanggungan orang tua, aset yang dimiliki, dan rekomendasi dari RT/RW.
-**Beasiswa Sponsor**
-Mahasiswa Sarjana Reguler UI juga mendapat kesempatan untuk memperoleh beasiswa dari pihak luar seperti pemerintah, bank, dan perusahaan swasta lainnya. Beasiswa yang diberikan beragam sifat maupun durasinya. Ada beasiswa yang hanya memberikan uang saku per bulan selama setahun, dan ada pula beasiswa yang memberikan uang saku bulanan ditambah dengan tunjangan BOP sampai mahasiswa tersebut lulus. Setiap tahunnya, sekitar 250 mahasiswa Sarjana Reguler Fasilkom dari seluruh angkatan mendapat beasiswa dari berbagai sponsor.</t>
-  </si>
-  <si>
-    <t>Beasiswa Fasilkom UI</t>
-  </si>
-  <si>
-    <t>**Pusat Ilmu Komputer Universitas Indonesia (Pusilkom UI)**
-Website: [https://www.pusilkom.ui.ac.id](https://www.pusilkom.ui.ac.id)
-Pusat Ilmu Komputer Universitas Indonesia (Pusilkom UI) didirikan pada tahun 1972 dengan latar belakang pembentukan untuk mengembangkan kompetensi civitas akademika Universitas Indonesia di bidang ilmu komputer. Sejak pembentukannya, Pusilkom UI telah aktif dalam mengembangkan ilmu komputer baik di dunia akademis, pemerintahan, maupun di dunia bisnis/industri.
-**Layanan Pusilkom UI**
-Sebagai unit usaha akademis dengan dukungan civitas akademika Fasilkom UI yang memiliki kompetensi di bidang ilmu komputer yang tidak diragukan lagi, Pusilkom UI menawarkan berbagai layanan di bidang teknologi informasi kepada kalangan industri, bisnis, dan pemerintah di Indonesia. Layanan-layanan tersebut meliputi training, konsultasi, pemrosesan data, pengembangan sistem informasi, dan riset.</t>
-  </si>
-  <si>
-    <t>Layanan Fasilkom UI</t>
-  </si>
-  <si>
-    <t>**Fakultas Ilmu Komputer Universitas Indonesia (Fasilkom UI)** adalah tempat yang menantang orang-orang dengan rasa ingin tahu yang tinggi dan bersemangat untuk berimajinasi dan berkarya di bidang ilmu komputer dan sistem informasi.
-Fasilkom UI merupakan salah satu institusi pendidikan tinggi terbaik di dunia dalam bidang ilmu komputer dan sistem informasi. Dengan riset yang mutakhir, start-up inovatif, ambisi yang besar, pembelajaran yang hands-on, dan robot-robot pintar, Fasilkom UI tidak hanya membayangkan masa depan, tapi juga turut membuatnya.
-- 2.800+ mahasiswa
-  - Terbaik dari seluruh penjuru nusantara
-- 80+ dosen
-  - Lulusan perguruan tinggi top dunia
-- 6.000+ alumni
-  - Dengan jaringan yang tersebar di tujuh benua</t>
-  </si>
-  <si>
-    <t>What is Fasilkom UI (Fakultas Ilmu Komputer Universitas Indonesia)</t>
+    <t>Apa saja layanan di Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa itu Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa saja persyaratan jalur masuk Fasilkom UI Doktor Ilmu Komputer (DIK)</t>
+  </si>
+  <si>
+    <t>Apa saja persyaratan jalur masuk Fasilkom UI Magister Teknologi Informasi (MTI) Double Degree</t>
+  </si>
+  <si>
+    <t>Apa saja persyaratan jalur masuk Fasilkom UI Magister Teknologi Informasi (MTI)</t>
+  </si>
+  <si>
+    <t>Apa saja persyaratan jalur masuk Fasilkom UI Magister Ilmu Komputer (MIK) Double Degree</t>
+  </si>
+  <si>
+    <t>Apa saja persyaratan jalur masuk Fasilkom UI Magister Ilmu Komputer (MIK)</t>
+  </si>
+  <si>
+    <t>Apa saja persyaratan jalur masuk Fasilkom UI kelas internasional (KKI)</t>
+  </si>
+  <si>
+    <t>Apa saja persyaratan jalur masuk Fasilkom UI sarjana Non Reguler (Non Reg)</t>
+  </si>
+  <si>
+    <t>Apa saja persyaratan jalur masuk Fasilkom UI sarjana Reguler (Reg)</t>
+  </si>
+  <si>
+    <t>Apa saja laboratorium dan pusat penelitian di Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa itu program pascasarjana Dokter Ilmu Komputer Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa itu program pascasarjana Magister Teknologi e-Government Informasi Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa itu program pascasarjana Magister Teknologi Informasi Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa itu program pascasarjana Magister Ilmu Komputer Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa itu program International Undergraduate Program in Computer Science/Information Technology di Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa itu program sarjana studi Sistem Informasi Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa itu program sarjana studi Ilmu Komputer Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa visi dan misi Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Bagaimana sejarah Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa saja achievements Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Apa saja divisi di RISTEK</t>
+  </si>
+  <si>
+    <t>Di mana lokasi RISTEK</t>
+  </si>
+  <si>
+    <t>Apa contact RISTEK</t>
+  </si>
+  <si>
+    <t>Apa saja projek RISTEK</t>
+  </si>
+  <si>
+    <t>Apa saja produk RISTEK</t>
+  </si>
+  <si>
+    <t>Apa itu RISTEK Ulas Kelas</t>
+  </si>
+  <si>
+    <t>Apa itu RISTEK susun jadwal</t>
+  </si>
+  <si>
+    <t>Apa itu RISTEK RISTEK.LINK</t>
+  </si>
+  <si>
+    <t>Apa saja RISTEK events</t>
+  </si>
+  <si>
+    <t>What are the benefits for RISTEK members</t>
+  </si>
+  <si>
+    <t>What are RISTEK achievements</t>
+  </si>
+  <si>
+    <t>What are RISTEK values</t>
+  </si>
+  <si>
+    <t>What are RISTEK services</t>
+  </si>
+  <si>
+    <t>What is the reason to collaborate with RISTEK</t>
+  </si>
+  <si>
+    <t>What are the benefits to collaborate with RISTEK</t>
+  </si>
+  <si>
+    <t>What is the primary goal of RISTEK</t>
+  </si>
+  <si>
+    <t>Apa saja persyaratan jalur masuk Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Bagaimana tata cara pendaftaran jalur masuk Fasilkom UI</t>
+  </si>
+  <si>
+    <t>Bagaimana tata cara pendaftaran jalur masuk Fasilkom UI sarjana Reguler (Reg)</t>
+  </si>
+  <si>
+    <t>Bagaimana tata cara pendaftaran jalur masuk Fasilkom UI sarjana Non Reguler (Non Reg)</t>
+  </si>
+  <si>
+    <t>Bagaimana tata cara pendaftaran jalur masuk Fasilkom UI kelas internasional (KKI)</t>
+  </si>
+  <si>
+    <t>Bagaimana tata cara pendaftaran jalur masuk Fasilkom UI Magister Ilmu Komputer (MIK)</t>
+  </si>
+  <si>
+    <t>Bagaimana tata cara pendaftaran jalur masuk Fasilkom UI Magister Ilmu Komputer (MIK) Double Degree</t>
+  </si>
+  <si>
+    <t>Bagaimana tata cara pendaftaran jalur masuk Fasilkom UI Magister Teknologi Informasi (MTI)</t>
+  </si>
+  <si>
+    <t>Bagaimana tata cara pendaftaran jalur masuk Fasilkom UI Magister Teknologi Informasi (MTI) Double Degree</t>
+  </si>
+  <si>
+    <t>Bagaimana tata cara pendaftaran jalur masuk Fasilkom UI Doktor Ilmu Komputer (DIK)</t>
   </si>
 </sst>
 </file>
@@ -1126,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7924FDD-4938-4597-972A-A9B3FA87D0C8}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1148,39 +1209,39 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1188,7 +1249,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1196,7 +1257,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -1204,226 +1265,354 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>